<commit_message>
Still processing BOM and updating library.
</commit_message>
<xml_diff>
--- a/hardware/PowerBoard/PowerBoard_BOM.xlsx
+++ b/hardware/PowerBoard/PowerBoard_BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="23955" windowHeight="14370"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="23955" windowHeight="14370" tabRatio="491"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="241">
   <si>
     <t>Item #</t>
   </si>
@@ -66,9 +66,6 @@
     <t>BEAD0603</t>
   </si>
   <si>
-    <t>BEAD</t>
-  </si>
-  <si>
     <t>C1</t>
   </si>
   <si>
@@ -255,9 +252,6 @@
     <t>INDUCTOR</t>
   </si>
   <si>
-    <t>LED0, LED1, LED2</t>
-  </si>
-  <si>
     <t>LED1208-RA</t>
   </si>
   <si>
@@ -595,16 +589,173 @@
   </si>
   <si>
     <t>Total Cost</t>
+  </si>
+  <si>
+    <t>Murata</t>
+  </si>
+  <si>
+    <t>490-5224-1-ND</t>
+  </si>
+  <si>
+    <t>BLM18SG700TN1D</t>
+  </si>
+  <si>
+    <t>FERRITE CHIP 70OHM 4A 0603</t>
+  </si>
+  <si>
+    <t>20mOhm@DC, 70Ohm@100MHz</t>
+  </si>
+  <si>
+    <t>TDK</t>
+  </si>
+  <si>
+    <t>C1608X7R1C154K</t>
+  </si>
+  <si>
+    <t>445-5123-1-ND</t>
+  </si>
+  <si>
+    <t>CAP CER .15UF 16V 10% X7R 0603</t>
+  </si>
+  <si>
+    <t>C1608X7R1C104K</t>
+  </si>
+  <si>
+    <t>445-1317-1-ND</t>
+  </si>
+  <si>
+    <t>CAP CER .10UF 16V 10% X7R 0603</t>
+  </si>
+  <si>
+    <t>CAP CER 10PF 50V C0G 5% 0603</t>
+  </si>
+  <si>
+    <t>C1608C0G1H100J</t>
+  </si>
+  <si>
+    <t>445-6852-1-ND</t>
+  </si>
+  <si>
+    <t>C1608X7R1C105K</t>
+  </si>
+  <si>
+    <t>CAP CER 1.0UF 16V X7R 10% 0603</t>
+  </si>
+  <si>
+    <t>445-1604-1-ND</t>
+  </si>
+  <si>
+    <t>C1608X7R1E103K</t>
+  </si>
+  <si>
+    <t>445-5100-1-ND</t>
+  </si>
+  <si>
+    <t>CAP CER 10000PF 25V X7R 10% 0603</t>
+  </si>
+  <si>
+    <t>CAP CER 4.0PF 50V C0G 0603</t>
+  </si>
+  <si>
+    <t>C1608C0G1H040B</t>
+  </si>
+  <si>
+    <t>445-5028-1-ND</t>
+  </si>
+  <si>
+    <t>CAP CER 10UF 6.3V X5R 20% 0603</t>
+  </si>
+  <si>
+    <t>C1608X5R0J106M</t>
+  </si>
+  <si>
+    <t>445-4112-1-ND</t>
+  </si>
+  <si>
+    <t>CAP CER 4.7UF 6.3V X5R 0603</t>
+  </si>
+  <si>
+    <t>C1608X5R0J475K</t>
+  </si>
+  <si>
+    <t>445-5178-1-ND</t>
+  </si>
+  <si>
+    <t>CONN MICRO SD R/A PUSH-PUSH SMD</t>
+  </si>
+  <si>
+    <t>CONN RCPT MICRO USB B SMD R/A</t>
+  </si>
+  <si>
+    <t>CONN HEADER 10 POS DUAL .05" SMD</t>
+  </si>
+  <si>
+    <t>CONN HEADER PH SIDE 2POS 2MM SMD</t>
+  </si>
+  <si>
+    <t>CONN JACK POWER 2.1MM PCB</t>
+  </si>
+  <si>
+    <t>CUI</t>
+  </si>
+  <si>
+    <t>CP-102A-ND</t>
+  </si>
+  <si>
+    <t>CONN PLUG 64POS VERT 1MM SMD</t>
+  </si>
+  <si>
+    <t>INDUCTOR POWER 1.6UH 1.7A SMD</t>
+  </si>
+  <si>
+    <t>LED1</t>
+  </si>
+  <si>
+    <t>LED0, LED2</t>
+  </si>
+  <si>
+    <t>GREEN</t>
+  </si>
+  <si>
+    <t>ORANGE</t>
+  </si>
+  <si>
+    <t>APECVA3010MGC</t>
+  </si>
+  <si>
+    <t>Kingbright</t>
+  </si>
+  <si>
+    <t>APECVA3010SECK</t>
+  </si>
+  <si>
+    <t>LED 3X1MM 601NM ORN RA CHIP SMD</t>
+  </si>
+  <si>
+    <t>754-1367-1-ND</t>
+  </si>
+  <si>
+    <t>754-1364-1-ND</t>
+  </si>
+  <si>
+    <t>LED 3.0X1.0MM 568NM GRN RA SMD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -633,12 +784,17 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -707,30 +863,39 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Output" xfId="1" builtinId="21"/>
+    <cellStyle name="Output" xfId="2" builtinId="21"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1022,26 +1187,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O57"/>
+  <dimension ref="A1:O58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.85546875" customWidth="1"/>
-    <col min="3" max="4" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" customWidth="1"/>
+    <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.140625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="32.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.140625" style="2"/>
     <col min="12" max="12" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="21">
       <c r="A1" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -1049,7 +1217,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
+      <c r="H1" s="8"/>
       <c r="I1" s="6"/>
       <c r="J1" s="8"/>
       <c r="K1" s="6"/>
@@ -1093,7 +1261,7 @@
         <v>9</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="M3" s="4" t="s">
         <v>11</v>
@@ -1112,17 +1280,32 @@
       <c r="B4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="2"/>
+      <c r="C4" s="2" t="s">
+        <v>195</v>
+      </c>
       <c r="D4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="I4" t="s">
+        <v>194</v>
+      </c>
       <c r="J4" s="2">
         <v>2</v>
       </c>
-      <c r="M4" t="s">
-        <v>16</v>
+      <c r="K4">
+        <v>0.35299999999999998</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -1130,21 +1313,37 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="I5" t="s">
+        <v>199</v>
+      </c>
+      <c r="J5" s="2">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>0.2</v>
+      </c>
+      <c r="M5" t="s">
         <v>19</v>
-      </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="J5" s="2">
-        <v>1</v>
-      </c>
-      <c r="M5" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -1152,21 +1351,37 @@
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="D6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+        <v>18</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="I6" t="s">
+        <v>202</v>
+      </c>
       <c r="J6" s="2">
         <v>5</v>
       </c>
+      <c r="K6">
+        <v>0.08</v>
+      </c>
       <c r="M6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -1174,21 +1389,37 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="D7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+        <v>18</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="I7" t="s">
+        <v>203</v>
+      </c>
       <c r="J7" s="2">
         <v>2</v>
       </c>
+      <c r="K7">
+        <v>0.12</v>
+      </c>
       <c r="M7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -1196,21 +1427,37 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="D8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="I8" t="s">
+        <v>207</v>
+      </c>
+      <c r="J8" s="2">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>0.23</v>
+      </c>
+      <c r="M8" t="s">
         <v>19</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="J8" s="2">
-        <v>1</v>
-      </c>
-      <c r="M8" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -1218,21 +1465,37 @@
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="D9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="I9" t="s">
+        <v>211</v>
+      </c>
+      <c r="J9" s="2">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>0.08</v>
+      </c>
+      <c r="M9" t="s">
         <v>19</v>
-      </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="J9" s="2">
-        <v>1</v>
-      </c>
-      <c r="M9" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:15">
@@ -1240,24 +1503,40 @@
         <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="D10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+        <v>18</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="I10" t="s">
+        <v>212</v>
+      </c>
       <c r="J10" s="2">
         <v>2</v>
       </c>
+      <c r="K10">
+        <v>0.16</v>
+      </c>
       <c r="M10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -1265,21 +1544,37 @@
         <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>33</v>
-      </c>
       <c r="D11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+        <v>18</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="I11" t="s">
+        <v>215</v>
+      </c>
       <c r="J11" s="2">
         <v>4</v>
       </c>
+      <c r="K11">
+        <v>0.46</v>
+      </c>
       <c r="M11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:15">
@@ -1287,21 +1582,37 @@
         <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="D12" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+        <v>18</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="I12" t="s">
+        <v>218</v>
+      </c>
       <c r="J12" s="2">
         <v>6</v>
       </c>
+      <c r="K12">
+        <v>0.36</v>
+      </c>
       <c r="M12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:15">
@@ -1309,31 +1620,37 @@
         <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="G13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
+        <v>221</v>
+      </c>
+      <c r="J13" s="2">
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <v>3.01</v>
+      </c>
+      <c r="M13" t="s">
         <v>41</v>
-      </c>
-      <c r="J13" s="2">
-        <v>1</v>
-      </c>
-      <c r="M13" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:15">
@@ -1341,31 +1658,37 @@
         <v>11</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="G14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I14" t="s">
+        <v>222</v>
+      </c>
+      <c r="J14" s="2">
+        <v>1</v>
+      </c>
+      <c r="K14">
+        <v>1.56</v>
+      </c>
+      <c r="M14" t="s">
         <v>44</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H14" t="s">
-        <v>46</v>
-      </c>
-      <c r="J14" s="2">
-        <v>1</v>
-      </c>
-      <c r="M14" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:15">
@@ -1373,31 +1696,37 @@
         <v>12</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E15" s="2" t="s">
+      <c r="F15" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="G15" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="H15" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="G15" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H15" t="s">
+      <c r="I15" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="J15" s="11">
+        <v>1</v>
+      </c>
+      <c r="K15" s="10">
+        <v>3.36</v>
+      </c>
+      <c r="M15" t="s">
         <v>51</v>
-      </c>
-      <c r="J15" s="2">
-        <v>1</v>
-      </c>
-      <c r="M15" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:15">
@@ -1405,31 +1734,37 @@
         <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E16" s="2" t="s">
+      <c r="F16" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="G16" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="H16" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="G16" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H16" t="s">
+      <c r="I16" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="J16" s="11">
+        <v>1</v>
+      </c>
+      <c r="K16" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="M16" t="s">
         <v>57</v>
-      </c>
-      <c r="J16" s="2">
-        <v>1</v>
-      </c>
-      <c r="M16" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:15">
@@ -1437,21 +1772,37 @@
         <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="D17" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="G17" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="I17" t="s">
+        <v>225</v>
+      </c>
+      <c r="J17" s="2">
+        <v>1</v>
+      </c>
+      <c r="K17">
+        <v>0.8</v>
+      </c>
+      <c r="M17" t="s">
         <v>60</v>
-      </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="J17" s="2">
-        <v>1</v>
-      </c>
-      <c r="M17" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:15">
@@ -1459,31 +1810,37 @@
         <v>15</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E18" s="2" t="s">
+      <c r="F18" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="G18" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H18" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="G18" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
+        <v>228</v>
+      </c>
+      <c r="J18" s="2">
+        <v>1</v>
+      </c>
+      <c r="K18">
+        <v>8.6</v>
+      </c>
+      <c r="M18" t="s">
         <v>66</v>
-      </c>
-      <c r="J18" s="2">
-        <v>1</v>
-      </c>
-      <c r="M18" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:15">
@@ -1491,13 +1848,13 @@
         <v>16</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>69</v>
-      </c>
       <c r="D19" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
@@ -1505,7 +1862,7 @@
         <v>1</v>
       </c>
       <c r="M19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:15">
@@ -1513,13 +1870,13 @@
         <v>17</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="D20" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
@@ -1527,7 +1884,7 @@
         <v>1</v>
       </c>
       <c r="M20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:15">
@@ -1535,29 +1892,37 @@
         <v>18</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="E21" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="F21" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2" t="s">
+      <c r="G21" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H21" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="G21" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H21" t="s">
+      <c r="I21" t="s">
+        <v>229</v>
+      </c>
+      <c r="J21" s="2">
+        <v>1</v>
+      </c>
+      <c r="K21">
+        <v>0.72</v>
+      </c>
+      <c r="M21" t="s">
         <v>77</v>
-      </c>
-      <c r="J21" s="2">
-        <v>1</v>
-      </c>
-      <c r="M21" t="s">
-        <v>78</v>
       </c>
       <c r="O21" s="3">
         <v>0.3</v>
@@ -1568,55 +1933,89 @@
         <v>19</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C22" s="2"/>
+        <v>231</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>233</v>
+      </c>
       <c r="D22" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
+        <v>78</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="I22" t="s">
+        <v>237</v>
+      </c>
       <c r="J22" s="2">
         <v>3</v>
       </c>
+      <c r="K22">
+        <v>0.28000000000000003</v>
+      </c>
       <c r="M22" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="1:15">
       <c r="A23">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>82</v>
+        <v>230</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>83</v>
+        <v>232</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
+        <v>78</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="I23" t="s">
+        <v>240</v>
+      </c>
       <c r="J23" s="2">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="K23">
+        <v>0.63</v>
       </c>
       <c r="M23" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="24" spans="1:15">
       <c r="A24">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
@@ -1624,156 +2023,156 @@
         <v>4</v>
       </c>
       <c r="M24" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:15">
       <c r="A25">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
-      <c r="G25" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H25" t="s">
-        <v>90</v>
-      </c>
       <c r="J25" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="M25" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="1:15">
       <c r="A26">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H26" t="s">
-        <v>94</v>
+        <v>39</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>88</v>
       </c>
       <c r="J26" s="2">
         <v>1</v>
       </c>
       <c r="M26" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:15">
       <c r="A27">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>99</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
       <c r="G27" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H27" t="s">
-        <v>94</v>
+        <v>39</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>92</v>
       </c>
       <c r="J27" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M27" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28" spans="1:15">
       <c r="A28">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C28" s="2">
-        <v>0</v>
+        <v>94</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>95</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
+        <v>95</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="J28" s="2">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M28" t="s">
-        <v>103</v>
-      </c>
-      <c r="O28" s="3">
-        <v>0.01</v>
+        <v>98</v>
       </c>
     </row>
     <row r="29" spans="1:15">
       <c r="A29">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>105</v>
+        <v>99</v>
+      </c>
+      <c r="C29" s="2">
+        <v>0</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="J29" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="M29" t="s">
-        <v>103</v>
+        <v>101</v>
+      </c>
+      <c r="O29" s="3">
+        <v>0.01</v>
       </c>
     </row>
     <row r="30" spans="1:15">
       <c r="A30">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>12</v>
+        <v>103</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
@@ -1781,21 +2180,21 @@
         <v>6</v>
       </c>
       <c r="M30" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="31" spans="1:15">
       <c r="A31">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>108</v>
+        <v>12</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
@@ -1803,46 +2202,46 @@
         <v>6</v>
       </c>
       <c r="M31" t="s">
-        <v>103</v>
-      </c>
-      <c r="O31" s="3">
-        <v>0.01</v>
+        <v>101</v>
       </c>
     </row>
     <row r="32" spans="1:15">
       <c r="A32">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="J32" s="2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="M32" t="s">
-        <v>103</v>
+        <v>101</v>
+      </c>
+      <c r="O32" s="3">
+        <v>0.01</v>
       </c>
     </row>
     <row r="33" spans="1:15">
       <c r="A33">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C33" s="2">
-        <v>120</v>
+        <v>107</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
@@ -1850,21 +2249,21 @@
         <v>1</v>
       </c>
       <c r="M33" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="34" spans="1:15">
       <c r="A34">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C34" s="2">
-        <v>330</v>
+        <v>120</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
@@ -1872,164 +2271,161 @@
         <v>1</v>
       </c>
       <c r="M34" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:15">
       <c r="A35">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C35" s="2">
-        <v>1</v>
+        <v>330</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
       <c r="J35" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M35" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="36" spans="1:15">
       <c r="A36">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
+      </c>
+      <c r="C36" s="2">
+        <v>1</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
       <c r="J36" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M36" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="37" spans="1:15">
       <c r="A37">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C37" s="2">
+        <v>112</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>102</v>
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
       <c r="J37" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M37" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="38" spans="1:15">
       <c r="A38">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C38" s="2">
-        <v>22</v>
+        <v>100</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
       <c r="J38" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M38" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="39" spans="1:15">
       <c r="A39">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C39" s="2">
-        <v>500</v>
+        <v>22</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
       <c r="J39" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M39" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="40" spans="1:15">
       <c r="A40">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>120</v>
+        <v>116</v>
+      </c>
+      <c r="C40" s="2">
+        <v>500</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
       <c r="J40" s="2">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="M40" t="s">
-        <v>103</v>
-      </c>
-      <c r="O40" s="3">
-        <v>0.01</v>
+        <v>101</v>
       </c>
     </row>
     <row r="41" spans="1:15">
       <c r="A41">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
       <c r="J41" s="2">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="M41" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="O41" s="3">
         <v>0.01</v>
@@ -2037,34 +2433,24 @@
     </row>
     <row r="42" spans="1:15">
       <c r="A42">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H42" t="s">
-        <v>127</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
       <c r="J42" s="2">
         <v>1</v>
       </c>
       <c r="M42" t="s">
-        <v>128</v>
+        <v>101</v>
       </c>
       <c r="O42" s="3">
         <v>0.01</v>
@@ -2072,38 +2458,51 @@
     </row>
     <row r="43" spans="1:15">
       <c r="A43">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
+        <v>122</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>125</v>
+      </c>
       <c r="J43" s="2">
         <v>1</v>
       </c>
       <c r="M43" t="s">
-        <v>132</v>
+        <v>126</v>
+      </c>
+      <c r="O43" s="3">
+        <v>0.01</v>
       </c>
     </row>
     <row r="44" spans="1:15">
       <c r="A44">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
@@ -2111,21 +2510,21 @@
         <v>1</v>
       </c>
       <c r="M44" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="45" spans="1:15">
       <c r="A45">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
@@ -2133,342 +2532,342 @@
         <v>1</v>
       </c>
       <c r="M45" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="46" spans="1:15">
       <c r="A46">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
       <c r="J46" s="2">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="M46" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="47" spans="1:15">
       <c r="A47">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="G47" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H47" t="s">
-        <v>146</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
       <c r="J47" s="2">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="M47" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="48" spans="1:15">
       <c r="A48">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H48" t="s">
-        <v>152</v>
+        <v>39</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>144</v>
       </c>
       <c r="J48" s="2">
         <v>1</v>
       </c>
       <c r="M48" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
     </row>
     <row r="49" spans="1:14">
       <c r="A49">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H49" t="s">
-        <v>157</v>
+        <v>39</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>150</v>
       </c>
       <c r="J49" s="2">
         <v>1</v>
       </c>
       <c r="M49" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
     </row>
     <row r="50" spans="1:14">
       <c r="A50">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="E50" s="2"/>
-      <c r="F50" s="2"/>
-      <c r="H50" t="s">
-        <v>161</v>
+        <v>153</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>155</v>
       </c>
       <c r="J50" s="2">
         <v>1</v>
       </c>
       <c r="M50" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="51" spans="1:14">
       <c r="A51">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="F51" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="G51" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H51" t="s">
-        <v>165</v>
+        <v>158</v>
+      </c>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="H51" s="2" t="s">
+        <v>159</v>
       </c>
       <c r="J51" s="2">
         <v>1</v>
       </c>
       <c r="M51" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="52" spans="1:14">
       <c r="A52">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>168</v>
+        <v>142</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H52" t="s">
-        <v>169</v>
+        <v>39</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="J52" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M52" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
     </row>
     <row r="53" spans="1:14">
       <c r="A53">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="E53" s="2"/>
-      <c r="F53" s="2"/>
+        <v>165</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>165</v>
+      </c>
       <c r="G53" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H53" t="s">
-        <v>173</v>
+        <v>39</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>167</v>
       </c>
       <c r="J53" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M53" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="54" spans="1:14">
       <c r="A54">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="F54" s="2" t="s">
-        <v>178</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
       <c r="G54" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H54" t="s">
-        <v>179</v>
+        <v>39</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>171</v>
       </c>
       <c r="J54" s="2">
         <v>1</v>
       </c>
       <c r="M54" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
     </row>
     <row r="55" spans="1:14">
       <c r="A55">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H55" t="s">
-        <v>185</v>
+        <v>39</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>177</v>
       </c>
       <c r="J55" s="2">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="M55" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
     </row>
     <row r="56" spans="1:14">
       <c r="A56">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="E56" s="2"/>
-      <c r="F56" s="2"/>
+        <v>180</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>183</v>
+      </c>
       <c r="J56" s="2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="M56" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="57" spans="1:14">
       <c r="A57">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
@@ -2476,10 +2875,32 @@
         <v>1</v>
       </c>
       <c r="M57" t="s">
-        <v>190</v>
-      </c>
-      <c r="N57" t="s">
-        <v>31</v>
+        <v>186</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14">
+      <c r="A58">
+        <v>54</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
+      <c r="J58" s="2">
+        <v>1</v>
+      </c>
+      <c r="M58" t="s">
+        <v>188</v>
+      </c>
+      <c r="N58" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor schematic, library and logo updates.
</commit_message>
<xml_diff>
--- a/hardware/PowerBoard/PowerBoard_BOM.xlsx
+++ b/hardware/PowerBoard/PowerBoard_BOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="311">
   <si>
     <t>Item #</t>
   </si>
@@ -960,6 +960,15 @@
       </rPr>
       <t xml:space="preserve"> This part does not require assembling</t>
     </r>
+  </si>
+  <si>
+    <t>Should DNP part value be noted?</t>
+  </si>
+  <si>
+    <t>Should DNP parts be ordered?</t>
+  </si>
+  <si>
+    <t>Should JUMPERS and FIDUCIALS be removed?</t>
   </si>
 </sst>
 </file>
@@ -1475,10 +1484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L65"/>
+  <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I2" sqref="I1:I1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H53" sqref="H53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3789,7 +3798,10 @@
         <v>5.15</v>
       </c>
     </row>
-    <row r="65" spans="9:12">
+    <row r="65" spans="2:12">
+      <c r="B65" s="9" t="s">
+        <v>309</v>
+      </c>
       <c r="I65" s="12" t="s">
         <v>304</v>
       </c>
@@ -3800,6 +3812,16 @@
       <c r="L65">
         <f>SUM(L4:L63)</f>
         <v>114.69000000000003</v>
+      </c>
+    </row>
+    <row r="66" spans="2:12">
+      <c r="B66" s="9" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="67" spans="2:12">
+      <c r="B67" s="9" t="s">
+        <v>310</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Library and BOM entries corrected for USBLC6-2 device (from SOT-666 to SOT23-6L)
</commit_message>
<xml_diff>
--- a/hardware/PowerBoard/PowerBoard_BOM.xlsx
+++ b/hardware/PowerBoard/PowerBoard_BOM.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="23955" windowHeight="14370" tabRatio="491"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="19440" windowHeight="12240" tabRatio="491"/>
   </bookViews>
   <sheets>
     <sheet name="Power Supply Board - Rev A" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -396,9 +396,6 @@
     <t>USBLC6-2</t>
   </si>
   <si>
-    <t>497-5026-1-ND</t>
-  </si>
-  <si>
     <t>U2</t>
   </si>
   <si>
@@ -849,12 +846,6 @@
     <t>IC FUEL/GAS GAUGE LI-ION 1A 6DFN</t>
   </si>
   <si>
-    <t>IC ESD PROTECTION FOR HS SOT-666</t>
-  </si>
-  <si>
-    <t>USBLC6-2P6</t>
-  </si>
-  <si>
     <t>IC USB POWER MANAGER 14-DFN</t>
   </si>
   <si>
@@ -919,13 +910,22 @@
   </si>
   <si>
     <t>NOTE: This part does not require assembling</t>
+  </si>
+  <si>
+    <t>497-5235-1-ND</t>
+  </si>
+  <si>
+    <t>USBLC6-2SC6</t>
+  </si>
+  <si>
+    <t>IC ESD PROTECTION LO CAP SOT23-6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1086,13 +1086,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Explanatory Text" xfId="2" builtinId="53"/>
@@ -1101,6 +1101,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1179,6 +1184,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1213,6 +1219,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1388,14 +1395,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C65" sqref="C65"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="37.140625" bestFit="1" customWidth="1"/>
@@ -1409,23 +1416,23 @@
     <col min="12" max="12" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="21">
-      <c r="A1" s="10" t="s">
-        <v>152</v>
-      </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-    </row>
-    <row r="3" spans="1:12" s="2" customFormat="1">
+    <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+    </row>
+    <row r="3" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -1460,10 +1467,10 @@
         <v>9</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -1471,25 +1478,25 @@
         <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="I4" t="s">
         <v>156</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="I4" t="s">
-        <v>157</v>
       </c>
       <c r="J4" s="2">
         <v>2</v>
@@ -1502,7 +1509,7 @@
         <v>0.70599999999999996</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="4" customFormat="1">
+    <row r="5" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>2</v>
       </c>
@@ -1516,19 +1523,19 @@
         <v>16</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F5" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="G5" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>177</v>
-      </c>
       <c r="I5" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J5" s="3">
         <v>2</v>
@@ -1541,7 +1548,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>3</v>
       </c>
@@ -1555,19 +1562,19 @@
         <v>16</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F6" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="G6" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>168</v>
-      </c>
       <c r="I6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J6" s="2">
         <v>2</v>
@@ -1580,7 +1587,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>4</v>
       </c>
@@ -1594,19 +1601,19 @@
         <v>16</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F7" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="G7" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H7" s="2" t="s">
+      <c r="I7" t="s">
         <v>173</v>
-      </c>
-      <c r="I7" t="s">
-        <v>174</v>
       </c>
       <c r="J7" s="2">
         <v>1</v>
@@ -1619,7 +1626,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>5</v>
       </c>
@@ -1633,19 +1640,19 @@
         <v>16</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F8" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H8" s="2" t="s">
+      <c r="I8" t="s">
         <v>164</v>
-      </c>
-      <c r="I8" t="s">
-        <v>165</v>
       </c>
       <c r="J8" s="2">
         <v>5</v>
@@ -1658,7 +1665,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>6</v>
       </c>
@@ -1672,19 +1679,19 @@
         <v>16</v>
       </c>
       <c r="E9" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="G9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H9" s="2" t="s">
+      <c r="I9" t="s">
         <v>161</v>
-      </c>
-      <c r="I9" t="s">
-        <v>162</v>
       </c>
       <c r="J9" s="2">
         <v>1</v>
@@ -1697,7 +1704,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>7</v>
       </c>
@@ -1711,19 +1718,19 @@
         <v>16</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F10" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="I10" t="s">
         <v>169</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="I10" t="s">
-        <v>170</v>
       </c>
       <c r="J10" s="2">
         <v>1</v>
@@ -1736,7 +1743,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>8</v>
       </c>
@@ -1750,19 +1757,19 @@
         <v>16</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F11" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="G11" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>183</v>
-      </c>
       <c r="I11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J11" s="2">
         <v>6</v>
@@ -1775,7 +1782,7 @@
         <v>2.16</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>9</v>
       </c>
@@ -1789,19 +1796,19 @@
         <v>16</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F12" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H12" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="G12" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>180</v>
-      </c>
       <c r="I12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J12" s="2">
         <v>4</v>
@@ -1814,7 +1821,7 @@
         <v>1.84</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>10</v>
       </c>
@@ -1840,7 +1847,7 @@
         <v>35</v>
       </c>
       <c r="I13" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J13" s="2">
         <v>1</v>
@@ -1853,7 +1860,7 @@
         <v>3.01</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>11</v>
       </c>
@@ -1879,7 +1886,7 @@
         <v>39</v>
       </c>
       <c r="I14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="J14" s="2">
         <v>1</v>
@@ -1892,7 +1899,7 @@
         <v>1.56</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>12</v>
       </c>
@@ -1918,7 +1925,7 @@
         <v>44</v>
       </c>
       <c r="I15" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J15" s="2">
         <v>1</v>
@@ -1931,12 +1938,12 @@
         <v>3.36</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>13</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>45</v>
@@ -1957,7 +1964,7 @@
         <v>48</v>
       </c>
       <c r="I16" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J16" s="2">
         <v>2</v>
@@ -1970,7 +1977,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>14</v>
       </c>
@@ -1984,7 +1991,7 @@
         <v>50</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>51</v>
@@ -1993,10 +2000,10 @@
         <v>34</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I17" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J17" s="2">
         <v>1</v>
@@ -2009,7 +2016,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>15</v>
       </c>
@@ -2035,7 +2042,7 @@
         <v>56</v>
       </c>
       <c r="I18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J18" s="2">
         <v>1</v>
@@ -2048,7 +2055,7 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="19" spans="1:12" s="4" customFormat="1">
+    <row r="19" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>16</v>
       </c>
@@ -2071,7 +2078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12" s="4" customFormat="1">
+    <row r="20" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>17</v>
       </c>
@@ -2094,7 +2101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>18</v>
       </c>
@@ -2108,7 +2115,7 @@
         <v>63</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>64</v>
@@ -2120,7 +2127,7 @@
         <v>65</v>
       </c>
       <c r="I21" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J21" s="2">
         <v>1</v>
@@ -2133,33 +2140,33 @@
         <v>0.72</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>19</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>66</v>
       </c>
       <c r="E22" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="F22" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="G22" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="I22" t="s">
         <v>199</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="I22" t="s">
-        <v>200</v>
       </c>
       <c r="J22" s="2">
         <v>3</v>
@@ -2172,33 +2179,33 @@
         <v>0.84000000000000008</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>20</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>66</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H23" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="I23" t="s">
         <v>202</v>
-      </c>
-      <c r="I23" t="s">
-        <v>203</v>
       </c>
       <c r="J23" s="2">
         <v>3</v>
@@ -2211,7 +2218,7 @@
         <v>1.8900000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>21</v>
       </c>
@@ -2234,7 +2241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>22</v>
       </c>
@@ -2257,7 +2264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>23</v>
       </c>
@@ -2274,7 +2281,7 @@
         <v>79</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>34</v>
@@ -2283,7 +2290,7 @@
         <v>73</v>
       </c>
       <c r="I26" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J26" s="2">
         <v>1</v>
@@ -2296,7 +2303,7 @@
         <v>0.76</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>24</v>
       </c>
@@ -2322,7 +2329,7 @@
         <v>76</v>
       </c>
       <c r="I27" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J27" s="2">
         <v>1</v>
@@ -2335,7 +2342,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>25</v>
       </c>
@@ -2352,16 +2359,16 @@
         <v>79</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I28" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="J28" s="2">
         <v>2</v>
@@ -2374,7 +2381,7 @@
         <v>1.68</v>
       </c>
     </row>
-    <row r="29" spans="1:12" s="4" customFormat="1">
+    <row r="29" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>26</v>
       </c>
@@ -2398,7 +2405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>27</v>
       </c>
@@ -2412,19 +2419,19 @@
         <v>82</v>
       </c>
       <c r="E30" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="F30" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="G30" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H30" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="G30" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H30" s="2" t="s">
+      <c r="I30" t="s">
         <v>213</v>
-      </c>
-      <c r="I30" t="s">
-        <v>214</v>
       </c>
       <c r="J30" s="2">
         <v>8</v>
@@ -2437,7 +2444,7 @@
         <v>0.14399999999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>28</v>
       </c>
@@ -2454,16 +2461,16 @@
         <v>79</v>
       </c>
       <c r="F31" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H31" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="G31" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H31" s="2" t="s">
+      <c r="I31" t="s">
         <v>216</v>
-      </c>
-      <c r="I31" t="s">
-        <v>217</v>
       </c>
       <c r="J31" s="2">
         <v>6</v>
@@ -2476,7 +2483,7 @@
         <v>7.92</v>
       </c>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>29</v>
       </c>
@@ -2490,19 +2497,19 @@
         <v>82</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F32" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="I32" t="s">
         <v>219</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="I32" t="s">
-        <v>220</v>
       </c>
       <c r="J32" s="2">
         <v>2</v>
@@ -2515,7 +2522,7 @@
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>30</v>
       </c>
@@ -2529,19 +2536,19 @@
         <v>82</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F33" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H33" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="G33" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H33" s="2" t="s">
+      <c r="I33" t="s">
         <v>222</v>
-      </c>
-      <c r="I33" t="s">
-        <v>223</v>
       </c>
       <c r="J33" s="2">
         <v>2</v>
@@ -2554,12 +2561,12 @@
         <v>4.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>31</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C34" s="2">
         <v>100</v>
@@ -2568,19 +2575,19 @@
         <v>82</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F34" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H34" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="G34" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H34" s="2" t="s">
+      <c r="I34" t="s">
         <v>226</v>
-      </c>
-      <c r="I34" t="s">
-        <v>227</v>
       </c>
       <c r="J34" s="2">
         <v>4</v>
@@ -2593,7 +2600,7 @@
         <v>7.1999999999999995E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>32</v>
       </c>
@@ -2607,19 +2614,19 @@
         <v>82</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G35" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H35" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="I35" t="s">
         <v>228</v>
-      </c>
-      <c r="I35" t="s">
-        <v>229</v>
       </c>
       <c r="J35" s="2">
         <v>1</v>
@@ -2632,7 +2639,7 @@
         <v>2.3E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>33</v>
       </c>
@@ -2646,19 +2653,19 @@
         <v>82</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F36" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H36" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="G36" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H36" s="2" t="s">
+      <c r="I36" t="s">
         <v>232</v>
-      </c>
-      <c r="I36" t="s">
-        <v>233</v>
       </c>
       <c r="J36" s="2">
         <v>1</v>
@@ -2671,7 +2678,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:12">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>34</v>
       </c>
@@ -2685,19 +2692,19 @@
         <v>82</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F37" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H37" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="G37" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H37" s="2" t="s">
+      <c r="I37" t="s">
         <v>235</v>
-      </c>
-      <c r="I37" t="s">
-        <v>236</v>
       </c>
       <c r="J37" s="2">
         <v>1</v>
@@ -2710,7 +2717,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:12">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>35</v>
       </c>
@@ -2724,19 +2731,19 @@
         <v>82</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F38" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H38" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="G38" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H38" s="2" t="s">
+      <c r="I38" t="s">
         <v>238</v>
-      </c>
-      <c r="I38" t="s">
-        <v>239</v>
       </c>
       <c r="J38" s="2">
         <v>1</v>
@@ -2749,7 +2756,7 @@
         <v>2.3E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>36</v>
       </c>
@@ -2763,19 +2770,19 @@
         <v>82</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F39" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H39" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="G39" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H39" s="2" t="s">
+      <c r="I39" t="s">
         <v>241</v>
-      </c>
-      <c r="I39" t="s">
-        <v>242</v>
       </c>
       <c r="J39" s="2">
         <v>6</v>
@@ -2788,7 +2795,7 @@
         <v>0.10799999999999998</v>
       </c>
     </row>
-    <row r="40" spans="1:12">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>37</v>
       </c>
@@ -2814,7 +2821,7 @@
         <v>104</v>
       </c>
       <c r="I40" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="J40" s="2">
         <v>1</v>
@@ -2827,7 +2834,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>38</v>
       </c>
@@ -2841,19 +2848,19 @@
         <v>82</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F41" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H41" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="G41" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H41" s="2" t="s">
+      <c r="I41" t="s">
         <v>245</v>
-      </c>
-      <c r="I41" t="s">
-        <v>246</v>
       </c>
       <c r="J41" s="2">
         <v>3</v>
@@ -2866,7 +2873,7 @@
         <v>6.9000000000000006E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:12">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>39</v>
       </c>
@@ -2880,19 +2887,19 @@
         <v>82</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F42" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H42" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="G42" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H42" s="2" t="s">
+      <c r="I42" t="s">
         <v>248</v>
-      </c>
-      <c r="I42" t="s">
-        <v>249</v>
       </c>
       <c r="J42" s="2">
         <v>9</v>
@@ -2905,7 +2912,7 @@
         <v>0.20699999999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:12">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>40</v>
       </c>
@@ -2919,19 +2926,19 @@
         <v>106</v>
       </c>
       <c r="E43" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H43" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="F43" s="2" t="s">
+      <c r="I43" t="s">
         <v>252</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H43" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="I43" t="s">
-        <v>253</v>
       </c>
       <c r="J43" s="2">
         <v>1</v>
@@ -2944,21 +2951,21 @@
         <v>5.45</v>
       </c>
     </row>
-    <row r="44" spans="1:12">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>41</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>109</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F44" s="2">
         <v>5122</v>
@@ -2967,10 +2974,10 @@
         <v>34</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I44" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="J44" s="2">
         <v>7</v>
@@ -2983,21 +2990,21 @@
         <v>2.66</v>
       </c>
     </row>
-    <row r="45" spans="1:12">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>42</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>109</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F45" s="2">
         <v>5121</v>
@@ -3006,10 +3013,10 @@
         <v>34</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="I45" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="J45" s="2">
         <v>2</v>
@@ -3022,21 +3029,21 @@
         <v>0.76</v>
       </c>
     </row>
-    <row r="46" spans="1:12">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>43</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>109</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F46" s="2">
         <v>5005</v>
@@ -3045,10 +3052,10 @@
         <v>34</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I46" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="J46" s="2">
         <v>1</v>
@@ -3061,21 +3068,21 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="47" spans="1:12">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>44</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>109</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F47" s="2">
         <v>5009</v>
@@ -3084,10 +3091,10 @@
         <v>34</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="I47" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="J47" s="2">
         <v>3</v>
@@ -3100,7 +3107,7 @@
         <v>1.08</v>
       </c>
     </row>
-    <row r="48" spans="1:12">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>45</v>
       </c>
@@ -3126,7 +3133,7 @@
         <v>114</v>
       </c>
       <c r="I48" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="J48" s="2">
         <v>1</v>
@@ -3139,7 +3146,7 @@
         <v>3.78</v>
       </c>
     </row>
-    <row r="49" spans="1:12">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>46</v>
       </c>
@@ -3165,7 +3172,7 @@
         <v>119</v>
       </c>
       <c r="I49" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="J49" s="2">
         <v>1</v>
@@ -3178,7 +3185,7 @@
         <v>8.9499999999999993</v>
       </c>
     </row>
-    <row r="50" spans="1:12">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>47</v>
       </c>
@@ -3204,7 +3211,7 @@
         <v>123</v>
       </c>
       <c r="I50" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="J50" s="2">
         <v>1</v>
@@ -3217,7 +3224,7 @@
         <v>4.51</v>
       </c>
     </row>
-    <row r="51" spans="1:12">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>48</v>
       </c>
@@ -3234,16 +3241,16 @@
         <v>117</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>278</v>
+        <v>299</v>
       </c>
       <c r="G51" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>126</v>
+        <v>298</v>
       </c>
       <c r="I51" t="s">
-        <v>277</v>
+        <v>300</v>
       </c>
       <c r="J51" s="2">
         <v>1</v>
@@ -3256,33 +3263,33 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:12">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>49</v>
       </c>
       <c r="B52" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C52" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="C52" s="2" t="s">
-        <v>128</v>
-      </c>
       <c r="D52" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>112</v>
       </c>
       <c r="F52" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H52" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="G52" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H52" s="2" t="s">
-        <v>130</v>
-      </c>
       <c r="I52" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="J52" s="2">
         <v>1</v>
@@ -3295,33 +3302,33 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="53" spans="1:12">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>50</v>
       </c>
       <c r="B53" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C53" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="D53" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E53" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="D53" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E53" s="2" t="s">
+      <c r="F53" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H53" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="F53" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="G53" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H53" s="2" t="s">
-        <v>134</v>
-      </c>
       <c r="I53" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="J53" s="2">
         <v>2</v>
@@ -3334,33 +3341,33 @@
         <v>1.76</v>
       </c>
     </row>
-    <row r="54" spans="1:12">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>51</v>
       </c>
       <c r="B54" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="D54" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H54" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="D54" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F54" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="G54" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H54" s="2" t="s">
-        <v>137</v>
-      </c>
       <c r="I54" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="J54" s="2">
         <v>1</v>
@@ -3373,33 +3380,33 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="55" spans="1:12">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>52</v>
       </c>
       <c r="B55" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C55" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="D55" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E55" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="D55" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="E55" s="2" t="s">
+      <c r="F55" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="F55" s="2" t="s">
+      <c r="G55" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H55" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="G55" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H55" s="2" t="s">
-        <v>142</v>
-      </c>
       <c r="I55" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="J55" s="2">
         <v>1</v>
@@ -3412,33 +3419,33 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="56" spans="1:12">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>53</v>
       </c>
       <c r="B56" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C56" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="D56" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E56" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="D56" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E56" s="2" t="s">
+      <c r="F56" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="F56" s="2" t="s">
+      <c r="G56" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H56" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="G56" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H56" s="2" t="s">
-        <v>147</v>
-      </c>
       <c r="I56" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="J56" s="2">
         <v>6</v>
@@ -3451,33 +3458,33 @@
         <v>10.08</v>
       </c>
     </row>
-    <row r="57" spans="1:12">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>54</v>
       </c>
       <c r="B57" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C57" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="C57" s="2" t="s">
-        <v>149</v>
-      </c>
       <c r="D57" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E57" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="I57" t="s">
         <v>284</v>
-      </c>
-      <c r="F57" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="G57" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H57" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="I57" t="s">
-        <v>287</v>
       </c>
       <c r="J57" s="2">
         <v>1</v>
@@ -3490,33 +3497,33 @@
         <v>3.45</v>
       </c>
     </row>
-    <row r="58" spans="1:12" s="4" customFormat="1">
+    <row r="58" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>55</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="G58" s="3" t="s">
         <v>34</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="I58" s="4" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="J58" s="3">
         <v>1</v>
@@ -3529,7 +3536,7 @@
         <v>1.26</v>
       </c>
     </row>
-    <row r="59" spans="1:12">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B59" s="8"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
@@ -3541,33 +3548,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:12" s="4" customFormat="1">
+    <row r="60" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>56</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="F60" s="3">
         <v>585460</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="H60" s="3" t="s">
-        <v>292</v>
-      </c>
-      <c r="I60" s="12" t="s">
-        <v>300</v>
+        <v>289</v>
+      </c>
+      <c r="I60" s="10" t="s">
+        <v>297</v>
       </c>
       <c r="J60" s="3">
         <v>1</v>
@@ -3580,21 +3587,21 @@
         <v>16.95</v>
       </c>
     </row>
-    <row r="61" spans="1:12" s="4" customFormat="1">
+    <row r="61" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>57</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F61" s="3">
         <v>8400</v>
@@ -3603,10 +3610,10 @@
         <v>34</v>
       </c>
       <c r="H61" s="3" t="s">
-        <v>296</v>
-      </c>
-      <c r="I61" s="12" t="s">
-        <v>300</v>
+        <v>293</v>
+      </c>
+      <c r="I61" s="10" t="s">
+        <v>297</v>
       </c>
       <c r="J61" s="3">
         <v>10</v>
@@ -3619,7 +3626,7 @@
         <v>5.15</v>
       </c>
     </row>
-    <row r="62" spans="1:12" s="4" customFormat="1">
+    <row r="62" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>58</v>
       </c>
@@ -3633,19 +3640,19 @@
         <v>108</v>
       </c>
       <c r="E62" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="G62" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H62" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="F62" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="G62" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="H62" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="I62" s="12" t="s">
-        <v>300</v>
+      <c r="I62" s="10" t="s">
+        <v>297</v>
       </c>
       <c r="J62" s="3">
         <v>1</v>
@@ -3658,9 +3665,9 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="63" spans="1:12">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I63" s="7" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="J63" s="2">
         <f>SUM(J4:J61)</f>
@@ -3681,24 +3688,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
- BOM - Gerber updated - Schematic pdf - Datasheet for connector
</commit_message>
<xml_diff>
--- a/hardware/PowerBoard/PowerBoard_BOM.xlsx
+++ b/hardware/PowerBoard/PowerBoard_BOM.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19440" windowHeight="12240" tabRatio="491"/>
+    <workbookView xWindow="0" yWindow="-165" windowWidth="22830" windowHeight="7185" tabRatio="491"/>
   </bookViews>
   <sheets>
     <sheet name="Power Supply Board - Rev A" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="301">
   <si>
     <t>Item #</t>
   </si>
@@ -177,30 +177,9 @@
     <t>J6</t>
   </si>
   <si>
-    <t>CON-71436-2164</t>
-  </si>
-  <si>
     <t>Molex</t>
   </si>
   <si>
-    <t>71436-2164</t>
-  </si>
-  <si>
-    <t>WM17200-ND</t>
-  </si>
-  <si>
-    <t>JP1</t>
-  </si>
-  <si>
-    <t>JUMPER-3PTH</t>
-  </si>
-  <si>
-    <t>JP2</t>
-  </si>
-  <si>
-    <t>JUMPER-2PTH-LOCK</t>
-  </si>
-  <si>
     <t>L1</t>
   </si>
   <si>
@@ -261,9 +240,6 @@
     <t>SI2312CDS-T1-GE3</t>
   </si>
   <si>
-    <t>R1, R12, R14, R21, R24, R25, R45, R48</t>
-  </si>
-  <si>
     <t>R0603</t>
   </si>
   <si>
@@ -273,42 +249,21 @@
     <t>4.7k</t>
   </si>
   <si>
-    <t>R13, R42, R43, R44, R51, R52</t>
-  </si>
-  <si>
-    <t>R15, R16, R17, R18, R19, R20</t>
-  </si>
-  <si>
     <t>50m</t>
   </si>
   <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>1k</t>
-  </si>
-  <si>
     <t>R23</t>
   </si>
   <si>
     <t>R26, R27</t>
   </si>
   <si>
-    <t>R3, R4, R8</t>
-  </si>
-  <si>
     <t>10k</t>
   </si>
   <si>
     <t>R49, R50</t>
   </si>
   <si>
-    <t>R5</t>
-  </si>
-  <si>
-    <t>R6, R10, R28, R30, R31, R40, R41, R46, R47</t>
-  </si>
-  <si>
     <t>100k</t>
   </si>
   <si>
@@ -342,9 +297,6 @@
     <t>SW3</t>
   </si>
   <si>
-    <t>SRB22A2</t>
-  </si>
-  <si>
     <t>TESTPOINT</t>
   </si>
   <si>
@@ -444,9 +396,6 @@
     <t>576-3228-1-ND</t>
   </si>
   <si>
-    <t>U7, U8, U9, U10, U11, U12</t>
-  </si>
-  <si>
     <t>MAX9938FEUK</t>
   </si>
   <si>
@@ -471,9 +420,6 @@
     <t>ECX-31B</t>
   </si>
   <si>
-    <t>Bill of Materials for 'Marote - Power Supply Board (Rev A)'</t>
-  </si>
-  <si>
     <t>Total Cost</t>
   </si>
   <si>
@@ -588,18 +534,12 @@
     <t>CP-102A-ND</t>
   </si>
   <si>
-    <t>CONN PLUG 64POS VERT 1MM SMD</t>
-  </si>
-  <si>
     <t>INDUCTOR POWER 1.6UH 1.7A SMD</t>
   </si>
   <si>
     <t>LED1</t>
   </si>
   <si>
-    <t>LED0, LED2</t>
-  </si>
-  <si>
     <t>GREEN</t>
   </si>
   <si>
@@ -708,24 +648,6 @@
     <t>MCR03EZPFX3300</t>
   </si>
   <si>
-    <t>MCR03EZPJ511</t>
-  </si>
-  <si>
-    <t>RHM510GCT-ND</t>
-  </si>
-  <si>
-    <t>RES 510 OHM 1/10W 5% 0603 SMD</t>
-  </si>
-  <si>
-    <t>MCR03EZPJ102</t>
-  </si>
-  <si>
-    <t>RHM1.0KGCT-ND</t>
-  </si>
-  <si>
-    <t>RES 1.0K OHM 1/10W 5% 0603 SMD</t>
-  </si>
-  <si>
     <t>MCR03EZPFX2101</t>
   </si>
   <si>
@@ -777,15 +699,6 @@
     <t>SW SLIDE SPDT 0.4VA GOLD R/A PC</t>
   </si>
   <si>
-    <t>Cherry</t>
-  </si>
-  <si>
-    <t>CH762-ND</t>
-  </si>
-  <si>
-    <t>SRB22A2BBWNN</t>
-  </si>
-  <si>
     <t>Keystone</t>
   </si>
   <si>
@@ -919,13 +832,100 @@
   </si>
   <si>
     <t>IC ESD PROTECTION LO CAP SOT23-6</t>
+  </si>
+  <si>
+    <t>Bill of Materials for 'Marote - Power Supply Board (Rev B)'</t>
+  </si>
+  <si>
+    <t>CON-71741-0002</t>
+  </si>
+  <si>
+    <t>71741-0002</t>
+  </si>
+  <si>
+    <t>WM3498CT-ND</t>
+  </si>
+  <si>
+    <t>MEZZANINE 1MM BTB PLUG 84CKT</t>
+  </si>
+  <si>
+    <t>LED2</t>
+  </si>
+  <si>
+    <t>R16, R17, R18, R19, R20</t>
+  </si>
+  <si>
+    <t>U8, U9, U10, U11, U12</t>
+  </si>
+  <si>
+    <t>SWITCH-ESWITCH-TL3340G</t>
+  </si>
+  <si>
+    <t>E-Switch</t>
+  </si>
+  <si>
+    <t>TL3340AF160QG</t>
+  </si>
+  <si>
+    <t>EG4627CT-ND</t>
+  </si>
+  <si>
+    <t>SWITCH TACTILE SPST-NO 0.05A 12V</t>
+  </si>
+  <si>
+    <t>J7</t>
+  </si>
+  <si>
+    <t>SWITCH-CJS-1200-1200</t>
+  </si>
+  <si>
+    <t>J-Lead</t>
+  </si>
+  <si>
+    <t>CJS</t>
+  </si>
+  <si>
+    <t>CJS-1200TA</t>
+  </si>
+  <si>
+    <t>563-1021-1-ND</t>
+  </si>
+  <si>
+    <t>CJS-1200 SPDT Switch</t>
+  </si>
+  <si>
+    <t>1.5k</t>
+  </si>
+  <si>
+    <t>R51</t>
+  </si>
+  <si>
+    <t>MCR03ERTF1501</t>
+  </si>
+  <si>
+    <t>RHM1.50KCFCT-ND</t>
+  </si>
+  <si>
+    <t>RES 1.50K OHM 1/10W 1% 0603 SMD</t>
+  </si>
+  <si>
+    <t>R6, R10, R28, R30, R31, R40, R41, R46, R47, R151, R152</t>
+  </si>
+  <si>
+    <t>R4, R8, R48</t>
+  </si>
+  <si>
+    <t>R13, R42, R43, R44, R212</t>
+  </si>
+  <si>
+    <t>R1, R12, R14, R211, R24, R25, R45, R451, R452, R453</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -971,12 +971,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1065,7 +1059,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1082,7 +1076,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1093,6 +1086,13 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Explanatory Text" xfId="2" builtinId="53"/>
@@ -1396,16 +1396,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L63"/>
+  <dimension ref="A1:L60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H51" sqref="H51"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.140625" customWidth="1"/>
     <col min="3" max="3" width="24.85546875" customWidth="1"/>
     <col min="4" max="4" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
@@ -1417,20 +1417,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
+      <c r="A1" s="10" t="s">
+        <v>272</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
     </row>
     <row r="3" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -1467,7 +1467,7 @@
         <v>9</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>152</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1478,25 +1478,25 @@
         <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>157</v>
+        <v>139</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="I4" t="s">
-        <v>156</v>
+        <v>138</v>
       </c>
       <c r="J4" s="2">
         <v>2</v>
@@ -1523,19 +1523,19 @@
         <v>16</v>
       </c>
       <c r="E5" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>176</v>
-      </c>
       <c r="I5" s="4" t="s">
-        <v>174</v>
+        <v>156</v>
       </c>
       <c r="J5" s="3">
         <v>2</v>
@@ -1544,7 +1544,7 @@
         <v>0.16</v>
       </c>
       <c r="L5" s="4">
-        <f t="shared" ref="L5:L61" si="0">J5*K5</f>
+        <f t="shared" ref="L5:L59" si="0">J5*K5</f>
         <v>0.32</v>
       </c>
     </row>
@@ -1562,19 +1562,19 @@
         <v>16</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>166</v>
+        <v>148</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>34</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
       <c r="I6" t="s">
-        <v>165</v>
+        <v>147</v>
       </c>
       <c r="J6" s="2">
         <v>2</v>
@@ -1601,19 +1601,19 @@
         <v>16</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>171</v>
+        <v>153</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>34</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>172</v>
+        <v>154</v>
       </c>
       <c r="I7" t="s">
-        <v>173</v>
+        <v>155</v>
       </c>
       <c r="J7" s="2">
         <v>1</v>
@@ -1640,19 +1640,19 @@
         <v>16</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>162</v>
+        <v>144</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
       <c r="I8" t="s">
-        <v>164</v>
+        <v>146</v>
       </c>
       <c r="J8" s="2">
         <v>5</v>
@@ -1679,19 +1679,19 @@
         <v>16</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>159</v>
+        <v>141</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="I9" t="s">
-        <v>161</v>
+        <v>143</v>
       </c>
       <c r="J9" s="2">
         <v>1</v>
@@ -1718,19 +1718,19 @@
         <v>16</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>168</v>
+        <v>150</v>
       </c>
       <c r="G10" s="6" t="s">
         <v>34</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>170</v>
+        <v>152</v>
       </c>
       <c r="I10" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="J10" s="2">
         <v>1</v>
@@ -1757,19 +1757,19 @@
         <v>16</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>181</v>
+        <v>163</v>
       </c>
       <c r="G11" s="6" t="s">
         <v>34</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>182</v>
+        <v>164</v>
       </c>
       <c r="I11" t="s">
-        <v>180</v>
+        <v>162</v>
       </c>
       <c r="J11" s="2">
         <v>6</v>
@@ -1796,19 +1796,19 @@
         <v>16</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>178</v>
+        <v>160</v>
       </c>
       <c r="G12" s="6" t="s">
         <v>34</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>179</v>
+        <v>161</v>
       </c>
       <c r="I12" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
       <c r="J12" s="2">
         <v>4</v>
@@ -1847,7 +1847,7 @@
         <v>35</v>
       </c>
       <c r="I13" t="s">
-        <v>183</v>
+        <v>165</v>
       </c>
       <c r="J13" s="2">
         <v>1</v>
@@ -1886,7 +1886,7 @@
         <v>39</v>
       </c>
       <c r="I14" t="s">
-        <v>184</v>
+        <v>166</v>
       </c>
       <c r="J14" s="2">
         <v>1</v>
@@ -1925,7 +1925,7 @@
         <v>44</v>
       </c>
       <c r="I15" t="s">
-        <v>185</v>
+        <v>167</v>
       </c>
       <c r="J15" s="2">
         <v>1</v>
@@ -1943,7 +1943,7 @@
         <v>13</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>296</v>
+        <v>267</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>45</v>
@@ -1964,7 +1964,7 @@
         <v>48</v>
       </c>
       <c r="I16" t="s">
-        <v>186</v>
+        <v>168</v>
       </c>
       <c r="J16" s="2">
         <v>2</v>
@@ -1991,7 +1991,7 @@
         <v>50</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>188</v>
+        <v>170</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>51</v>
@@ -2000,10 +2000,10 @@
         <v>34</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>189</v>
+        <v>171</v>
       </c>
       <c r="I17" t="s">
-        <v>187</v>
+        <v>169</v>
       </c>
       <c r="J17" s="2">
         <v>1</v>
@@ -2024,81 +2024,113 @@
         <v>52</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="F18" s="2" t="s">
-        <v>55</v>
+        <v>274</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="I18" t="s">
-        <v>190</v>
+        <v>275</v>
+      </c>
+      <c r="I18" s="12" t="s">
+        <v>276</v>
       </c>
       <c r="J18" s="2">
         <v>1</v>
       </c>
       <c r="K18">
-        <v>8.6</v>
+        <v>6.24</v>
       </c>
       <c r="L18">
         <f t="shared" si="0"/>
-        <v>8.6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
+        <v>6.24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
         <v>16</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>286</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="I19" s="12" t="s">
+        <v>291</v>
+      </c>
+      <c r="J19" s="2">
+        <v>1</v>
+      </c>
+      <c r="K19">
+        <v>0.97</v>
+      </c>
+      <c r="L19">
+        <f t="shared" ref="L19" si="1">J19*K19</f>
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>17</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="3" t="s">
+      <c r="G20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H20" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="J19" s="3">
+      <c r="I20" t="s">
+        <v>172</v>
+      </c>
+      <c r="J20" s="2">
         <v>1</v>
       </c>
-      <c r="L19" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
-        <v>17</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="J20" s="3">
-        <v>1</v>
-      </c>
-      <c r="L20" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="K20">
+        <v>0.72</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="0"/>
+        <v>0.72</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -2106,38 +2138,38 @@
         <v>18</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>61</v>
+        <v>277</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>62</v>
+        <v>175</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>158</v>
+        <v>177</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>64</v>
+        <v>178</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>65</v>
+        <v>180</v>
       </c>
       <c r="I21" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="J21" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K21">
-        <v>0.72</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="L21">
         <f t="shared" si="0"/>
-        <v>0.72</v>
+        <v>0.84000000000000008</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -2145,38 +2177,38 @@
         <v>19</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>193</v>
+        <v>173</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>197</v>
+        <v>177</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>198</v>
+        <v>176</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>200</v>
+        <v>181</v>
       </c>
       <c r="I22" t="s">
-        <v>199</v>
+        <v>182</v>
       </c>
       <c r="J22" s="2">
         <v>3</v>
       </c>
       <c r="K22">
-        <v>0.28000000000000003</v>
+        <v>0.63</v>
       </c>
       <c r="L22">
         <f t="shared" si="0"/>
-        <v>0.84000000000000008</v>
+        <v>1.8900000000000001</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -2184,38 +2216,22 @@
         <v>20</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>192</v>
+        <v>60</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>194</v>
+        <v>61</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="I23" t="s">
-        <v>202</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
       <c r="J23" s="2">
-        <v>3</v>
-      </c>
-      <c r="K23">
-        <v>0.63</v>
+        <v>4</v>
       </c>
       <c r="L23">
         <f t="shared" si="0"/>
-        <v>1.8900000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -2223,13 +2239,13 @@
         <v>21</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
@@ -2246,22 +2262,38 @@
         <v>22</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
+        <v>65</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I25" t="s">
+        <v>186</v>
+      </c>
       <c r="J25" s="2">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="K25">
+        <v>0.76</v>
       </c>
       <c r="L25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -2269,38 +2301,38 @@
         <v>23</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C26" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="F26" s="2" t="s">
-        <v>205</v>
+        <v>73</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I26" t="s">
-        <v>206</v>
+        <v>187</v>
       </c>
       <c r="J26" s="2">
         <v>1</v>
       </c>
       <c r="K26">
-        <v>0.76</v>
+        <v>0.45</v>
       </c>
       <c r="L26">
         <f t="shared" si="0"/>
-        <v>0.76</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -2308,101 +2340,101 @@
         <v>24</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="I27" t="s">
+        <v>188</v>
+      </c>
+      <c r="J27" s="2">
+        <v>2</v>
+      </c>
+      <c r="K27">
+        <v>0.84</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="0"/>
+        <v>1.68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
+        <v>25</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="I27" t="s">
-        <v>207</v>
-      </c>
-      <c r="J27" s="2">
-        <v>1</v>
-      </c>
-      <c r="K27">
-        <v>0.45</v>
-      </c>
-      <c r="L27">
-        <f t="shared" si="0"/>
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
-        <v>25</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="I28" t="s">
-        <v>208</v>
-      </c>
-      <c r="J28" s="2">
-        <v>2</v>
-      </c>
-      <c r="K28">
-        <v>0.84</v>
-      </c>
-      <c r="L28">
-        <f t="shared" si="0"/>
-        <v>1.68</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="3">
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="J28" s="3">
+        <v>6</v>
+      </c>
+      <c r="L28" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
         <v>26</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="J29" s="3">
-        <v>6</v>
-      </c>
-      <c r="L29" s="4">
-        <f t="shared" si="0"/>
+      <c r="B29" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="C29" s="2">
         <v>0</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="I29" t="s">
+        <v>193</v>
+      </c>
+      <c r="J29" s="2">
+        <v>8</v>
+      </c>
+      <c r="K29">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="0"/>
+        <v>0.14399999999999999</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -2410,38 +2442,38 @@
         <v>27</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C30" s="2">
-        <v>0</v>
+        <v>278</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>210</v>
+        <v>72</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>211</v>
+        <v>194</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>212</v>
+        <v>195</v>
       </c>
       <c r="I30" t="s">
-        <v>213</v>
+        <v>196</v>
       </c>
       <c r="J30" s="2">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K30">
-        <v>1.7999999999999999E-2</v>
+        <v>1.32</v>
       </c>
       <c r="L30">
         <f t="shared" si="0"/>
-        <v>0.14399999999999999</v>
+        <v>7.92</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -2449,38 +2481,38 @@
         <v>28</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>87</v>
+        <v>79</v>
+      </c>
+      <c r="C31" s="2">
+        <v>1</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>79</v>
+        <v>190</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>214</v>
+        <v>198</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>215</v>
+        <v>197</v>
       </c>
       <c r="I31" t="s">
-        <v>216</v>
+        <v>199</v>
       </c>
       <c r="J31" s="2">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="K31">
-        <v>1.32</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="L31">
         <f t="shared" si="0"/>
-        <v>7.92</v>
+        <v>3.5999999999999997E-2</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -2488,38 +2520,38 @@
         <v>29</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="C32" s="2">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>210</v>
+        <v>190</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>218</v>
+        <v>200</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>217</v>
+        <v>201</v>
       </c>
       <c r="I32" t="s">
-        <v>219</v>
+        <v>202</v>
       </c>
       <c r="J32" s="2">
         <v>2</v>
       </c>
       <c r="K32">
-        <v>1.7999999999999999E-2</v>
+        <v>2.3E-2</v>
       </c>
       <c r="L32">
         <f t="shared" si="0"/>
-        <v>3.5999999999999997E-2</v>
+        <v>4.5999999999999999E-2</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
@@ -2527,38 +2559,38 @@
         <v>30</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>94</v>
+        <v>203</v>
       </c>
       <c r="C33" s="2">
-        <v>22</v>
+        <v>100</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>210</v>
+        <v>190</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>220</v>
+        <v>204</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>221</v>
+        <v>205</v>
       </c>
       <c r="I33" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
       <c r="J33" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K33">
-        <v>2.3E-2</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="L33">
         <f t="shared" si="0"/>
-        <v>4.5999999999999999E-2</v>
+        <v>7.1999999999999995E-2</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
@@ -2566,38 +2598,38 @@
         <v>31</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>223</v>
+        <v>78</v>
       </c>
       <c r="C34" s="2">
-        <v>100</v>
+        <v>330</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>210</v>
+        <v>190</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
       <c r="G34" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>225</v>
+        <v>207</v>
       </c>
       <c r="I34" t="s">
-        <v>226</v>
+        <v>208</v>
       </c>
       <c r="J34" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K34">
-        <v>1.7999999999999999E-2</v>
+        <v>2.3E-2</v>
       </c>
       <c r="L34">
         <f t="shared" si="0"/>
-        <v>7.1999999999999995E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
@@ -2605,38 +2637,38 @@
         <v>32</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C35" s="2">
-        <v>330</v>
+        <v>293</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>292</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>210</v>
+        <v>190</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>229</v>
+        <v>294</v>
       </c>
       <c r="G35" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="I35" t="s">
-        <v>228</v>
+        <v>295</v>
+      </c>
+      <c r="I35" s="14" t="s">
+        <v>296</v>
       </c>
       <c r="J35" s="2">
         <v>1</v>
       </c>
       <c r="K35">
-        <v>2.3E-2</v>
+        <v>0.21</v>
       </c>
       <c r="L35">
         <f t="shared" si="0"/>
-        <v>2.3E-2</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
@@ -2644,38 +2676,38 @@
         <v>33</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C36" s="2">
-        <v>510</v>
+        <v>83</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>84</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="E36" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F36" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="F36" s="2" t="s">
-        <v>230</v>
-      </c>
       <c r="G36" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>231</v>
+        <v>211</v>
       </c>
       <c r="I36" t="s">
-        <v>232</v>
+        <v>212</v>
       </c>
       <c r="J36" s="2">
         <v>1</v>
       </c>
       <c r="K36">
-        <v>1.7999999999999999E-2</v>
+        <v>2.3E-2</v>
       </c>
       <c r="L36">
         <f t="shared" si="0"/>
-        <v>1.7999999999999999E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
@@ -2683,38 +2715,38 @@
         <v>34</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>210</v>
+        <v>190</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>233</v>
+        <v>213</v>
       </c>
       <c r="G37" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>234</v>
+        <v>214</v>
       </c>
       <c r="I37" t="s">
-        <v>235</v>
+        <v>215</v>
       </c>
       <c r="J37" s="2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="K37">
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="L37">
         <f t="shared" si="0"/>
-        <v>1.7999999999999999E-2</v>
+        <v>0.10799999999999998</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
@@ -2722,38 +2754,38 @@
         <v>35</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>210</v>
+        <v>87</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>236</v>
+        <v>88</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>237</v>
+        <v>89</v>
       </c>
       <c r="I38" t="s">
-        <v>238</v>
+        <v>216</v>
       </c>
       <c r="J38" s="2">
         <v>1</v>
       </c>
       <c r="K38">
-        <v>2.3E-2</v>
+        <v>1</v>
       </c>
       <c r="L38">
         <f t="shared" si="0"/>
-        <v>2.3E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
@@ -2761,38 +2793,38 @@
         <v>36</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>83</v>
+        <v>298</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>210</v>
+        <v>190</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>239</v>
+        <v>217</v>
       </c>
       <c r="G39" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>240</v>
+        <v>218</v>
       </c>
       <c r="I39" t="s">
-        <v>241</v>
+        <v>219</v>
       </c>
       <c r="J39" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="K39">
-        <v>1.7999999999999999E-2</v>
+        <v>2.3E-2</v>
       </c>
       <c r="L39">
         <f t="shared" si="0"/>
-        <v>0.10799999999999998</v>
+        <v>6.9000000000000006E-2</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
@@ -2800,38 +2832,38 @@
         <v>37</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>100</v>
+        <v>297</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>101</v>
+        <v>74</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>102</v>
+        <v>190</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>103</v>
+        <v>220</v>
       </c>
       <c r="G40" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>104</v>
+        <v>221</v>
       </c>
       <c r="I40" t="s">
-        <v>242</v>
+        <v>222</v>
       </c>
       <c r="J40" s="2">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="K40">
-        <v>1</v>
+        <v>2.3E-2</v>
       </c>
       <c r="L40">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.20699999999999999</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
@@ -2839,38 +2871,38 @@
         <v>38</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>210</v>
+        <v>223</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>243</v>
+        <v>225</v>
       </c>
       <c r="G41" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>244</v>
+        <v>224</v>
       </c>
       <c r="I41" t="s">
-        <v>245</v>
+        <v>226</v>
       </c>
       <c r="J41" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K41">
-        <v>2.3E-2</v>
+        <v>5.45</v>
       </c>
       <c r="L41">
         <f t="shared" si="0"/>
-        <v>6.9000000000000006E-2</v>
+        <v>5.45</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
@@ -2878,77 +2910,77 @@
         <v>39</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>280</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>82</v>
+        <v>280</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>210</v>
+        <v>281</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>246</v>
+        <v>282</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="I42" t="s">
-        <v>248</v>
+        <v>283</v>
+      </c>
+      <c r="I42" s="12" t="s">
+        <v>284</v>
       </c>
       <c r="J42" s="2">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="K42">
-        <v>2.3E-2</v>
+        <v>0.29099999999999998</v>
       </c>
       <c r="L42">
-        <f t="shared" si="0"/>
-        <v>0.20699999999999999</v>
+        <f t="shared" ref="L42" si="2">J42*K42</f>
+        <v>0.29099999999999998</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>40</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>105</v>
+      <c r="B43" s="7" t="s">
+        <v>228</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>106</v>
+        <v>229</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>251</v>
+        <v>227</v>
+      </c>
+      <c r="F43" s="2">
+        <v>5122</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="I43" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="J43" s="2">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="K43">
-        <v>5.45</v>
+        <v>0.38</v>
       </c>
       <c r="L43">
         <f t="shared" si="0"/>
-        <v>5.45</v>
+        <v>2.66</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
@@ -2956,38 +2988,38 @@
         <v>41</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>257</v>
+        <v>230</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>258</v>
+        <v>231</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>256</v>
+        <v>227</v>
       </c>
       <c r="F44" s="2">
-        <v>5122</v>
+        <v>5121</v>
       </c>
       <c r="G44" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>265</v>
+        <v>237</v>
       </c>
       <c r="I44" t="s">
-        <v>269</v>
+        <v>241</v>
       </c>
       <c r="J44" s="2">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="K44">
         <v>0.38</v>
       </c>
       <c r="L44">
         <f t="shared" si="0"/>
-        <v>2.66</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
@@ -2995,38 +3027,38 @@
         <v>42</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>259</v>
+        <v>232</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>260</v>
+        <v>233</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>256</v>
+        <v>227</v>
       </c>
       <c r="F45" s="2">
-        <v>5121</v>
+        <v>5005</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>266</v>
+        <v>238</v>
       </c>
       <c r="I45" t="s">
-        <v>270</v>
+        <v>242</v>
       </c>
       <c r="J45" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K45">
-        <v>0.38</v>
+        <v>0.36</v>
       </c>
       <c r="L45">
         <f t="shared" si="0"/>
-        <v>0.76</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
@@ -3034,77 +3066,77 @@
         <v>43</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>261</v>
+        <v>234</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>262</v>
+        <v>235</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>256</v>
+        <v>227</v>
       </c>
       <c r="F46" s="2">
-        <v>5005</v>
+        <v>5009</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>267</v>
+        <v>239</v>
       </c>
       <c r="I46" t="s">
-        <v>271</v>
+        <v>243</v>
       </c>
       <c r="J46" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K46">
         <v>0.36</v>
       </c>
       <c r="L46">
         <f t="shared" si="0"/>
-        <v>0.36</v>
+        <v>1.08</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>44</v>
       </c>
-      <c r="B47" s="7" t="s">
-        <v>263</v>
+      <c r="B47" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>264</v>
+        <v>95</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="F47" s="2">
-        <v>5009</v>
+        <v>96</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>268</v>
+        <v>98</v>
       </c>
       <c r="I47" t="s">
-        <v>272</v>
+        <v>244</v>
       </c>
       <c r="J47" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K47">
-        <v>0.36</v>
+        <v>3.78</v>
       </c>
       <c r="L47">
         <f t="shared" si="0"/>
-        <v>1.08</v>
+        <v>3.78</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
@@ -3112,38 +3144,38 @@
         <v>45</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="G48" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="I48" t="s">
-        <v>273</v>
+        <v>245</v>
       </c>
       <c r="J48" s="2">
         <v>1</v>
       </c>
       <c r="K48">
-        <v>3.78</v>
+        <v>8.9499999999999993</v>
       </c>
       <c r="L48">
         <f t="shared" si="0"/>
-        <v>3.78</v>
+        <v>8.9499999999999993</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
@@ -3151,38 +3183,38 @@
         <v>46</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="G49" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="I49" t="s">
-        <v>274</v>
+        <v>246</v>
       </c>
       <c r="J49" s="2">
         <v>1</v>
       </c>
       <c r="K49">
-        <v>8.9499999999999993</v>
+        <v>4.51</v>
       </c>
       <c r="L49">
         <f t="shared" si="0"/>
-        <v>8.9499999999999993</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
@@ -3190,38 +3222,38 @@
         <v>47</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>122</v>
+        <v>270</v>
       </c>
       <c r="G50" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>123</v>
+        <v>269</v>
       </c>
       <c r="I50" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="J50" s="2">
         <v>1</v>
       </c>
       <c r="K50">
-        <v>4.51</v>
+        <v>1</v>
       </c>
       <c r="L50">
         <f t="shared" si="0"/>
-        <v>4.51</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
@@ -3229,38 +3261,38 @@
         <v>48</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>299</v>
+        <v>112</v>
       </c>
       <c r="G51" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>298</v>
+        <v>113</v>
       </c>
       <c r="I51" t="s">
-        <v>300</v>
+        <v>247</v>
       </c>
       <c r="J51" s="2">
         <v>1</v>
       </c>
       <c r="K51">
-        <v>1</v>
+        <v>3.3</v>
       </c>
       <c r="L51">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
@@ -3268,38 +3300,38 @@
         <v>49</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="G52" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="I52" t="s">
-        <v>276</v>
+        <v>248</v>
       </c>
       <c r="J52" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K52">
-        <v>3.3</v>
+        <v>0.88</v>
       </c>
       <c r="L52">
         <f t="shared" si="0"/>
-        <v>3.3</v>
+        <v>1.76</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
@@ -3307,38 +3339,38 @@
         <v>50</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="G53" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="I53" t="s">
-        <v>277</v>
+        <v>249</v>
       </c>
       <c r="J53" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K53">
-        <v>0.88</v>
+        <v>1.5</v>
       </c>
       <c r="L53">
         <f t="shared" si="0"/>
-        <v>1.76</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
@@ -3346,38 +3378,38 @@
         <v>51</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="G54" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="I54" t="s">
-        <v>278</v>
+        <v>250</v>
       </c>
       <c r="J54" s="2">
         <v>1</v>
       </c>
       <c r="K54">
-        <v>1.5</v>
+        <v>1.3</v>
       </c>
       <c r="L54">
         <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
@@ -3385,38 +3417,38 @@
         <v>52</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>137</v>
+        <v>279</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="G55" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="I55" t="s">
-        <v>279</v>
+        <v>251</v>
       </c>
       <c r="J55" s="2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="K55">
-        <v>1.3</v>
+        <v>1.68</v>
       </c>
       <c r="L55">
         <f t="shared" si="0"/>
-        <v>1.3</v>
+        <v>10.08</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
@@ -3424,77 +3456,77 @@
         <v>53</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>144</v>
+        <v>252</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>145</v>
+        <v>253</v>
       </c>
       <c r="G56" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>146</v>
+        <v>254</v>
       </c>
       <c r="I56" t="s">
-        <v>280</v>
+        <v>255</v>
       </c>
       <c r="J56" s="2">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="K56">
-        <v>1.68</v>
+        <v>3.45</v>
       </c>
       <c r="L56">
         <f t="shared" si="0"/>
-        <v>10.08</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A57" s="2">
+        <v>3.45</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="3">
         <v>54</v>
       </c>
-      <c r="B57" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="F57" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="G57" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H57" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="I57" t="s">
-        <v>284</v>
-      </c>
-      <c r="J57" s="2">
+      <c r="B57" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H57" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="I57" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="J57" s="3">
         <v>1</v>
       </c>
-      <c r="K57">
-        <v>3.45</v>
-      </c>
-      <c r="L57">
-        <f t="shared" si="0"/>
-        <v>3.45</v>
+      <c r="K57" s="4">
+        <v>1.26</v>
+      </c>
+      <c r="L57" s="4">
+        <f t="shared" si="0"/>
+        <v>1.26</v>
       </c>
     </row>
     <row r="58" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -3502,180 +3534,90 @@
         <v>55</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>149</v>
+        <v>189</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>150</v>
+        <v>262</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="F58" s="3" t="s">
-        <v>285</v>
+        <v>261</v>
+      </c>
+      <c r="F58" s="3">
+        <v>585460</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>34</v>
+        <v>259</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I58" s="4" t="s">
-        <v>287</v>
+        <v>260</v>
+      </c>
+      <c r="I58" s="9" t="s">
+        <v>268</v>
       </c>
       <c r="J58" s="3">
         <v>1</v>
       </c>
       <c r="K58" s="4">
-        <v>1.26</v>
+        <v>16.95</v>
       </c>
       <c r="L58" s="4">
         <f t="shared" si="0"/>
-        <v>1.26</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B59" s="8"/>
-      <c r="C59" s="2"/>
-      <c r="D59" s="2"/>
-      <c r="E59" s="2"/>
-      <c r="F59" s="2"/>
-      <c r="G59" s="2"/>
-      <c r="L59">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="3">
+        <v>16.95</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="3">
         <v>56</v>
       </c>
-      <c r="B60" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="C60" s="3" t="s">
+      <c r="B59" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="C59" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D60" s="3" t="s">
-        <v>291</v>
-      </c>
-      <c r="E60" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="F60" s="3">
-        <v>585460</v>
-      </c>
-      <c r="G60" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="H60" s="3" t="s">
-        <v>289</v>
-      </c>
-      <c r="I60" s="10" t="s">
-        <v>297</v>
-      </c>
-      <c r="J60" s="3">
-        <v>1</v>
-      </c>
-      <c r="K60" s="4">
-        <v>16.95</v>
-      </c>
-      <c r="L60" s="4">
-        <f t="shared" si="0"/>
-        <v>16.95</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="3">
-        <v>57</v>
-      </c>
-      <c r="B61" s="4" t="s">
-        <v>292</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>295</v>
-      </c>
-      <c r="E61" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="F61" s="3">
+      <c r="D59" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="F59" s="3">
         <v>8400</v>
       </c>
-      <c r="G61" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="H61" s="3" t="s">
-        <v>293</v>
-      </c>
-      <c r="I61" s="10" t="s">
-        <v>297</v>
-      </c>
-      <c r="J61" s="3">
+      <c r="G59" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H59" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I59" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="J59" s="3">
         <v>10</v>
       </c>
-      <c r="K61" s="4">
+      <c r="K59" s="4">
         <v>0.51500000000000001</v>
       </c>
-      <c r="L61" s="4">
+      <c r="L59" s="4">
         <f t="shared" si="0"/>
         <v>5.15</v>
       </c>
     </row>
-    <row r="62" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="3">
-        <v>58</v>
-      </c>
-      <c r="B62" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="E62" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="F62" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="G62" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="H62" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="I62" s="10" t="s">
-        <v>297</v>
-      </c>
-      <c r="J62" s="3">
-        <v>1</v>
-      </c>
-      <c r="K62" s="4">
-        <v>0.86</v>
-      </c>
-      <c r="L62" s="4">
-        <f t="shared" ref="L62" si="1">J62*K62</f>
-        <v>0.86</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I63" s="7" t="s">
-        <v>294</v>
-      </c>
-      <c r="J63" s="2">
-        <f>SUM(J4:J61)</f>
-        <v>145</v>
-      </c>
-      <c r="L63">
-        <f>SUM(L4:L61)</f>
-        <v>113.83000000000003</v>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I60" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="J60" s="2">
+        <f>SUM(J4:J59)</f>
+        <v>144</v>
+      </c>
+      <c r="L60">
+        <f>SUM(L4:L59)</f>
+        <v>112.90500000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Removed some components from BOM
</commit_message>
<xml_diff>
--- a/hardware/PowerBoard/PowerBoard_BOM.xlsx
+++ b/hardware/PowerBoard/PowerBoard_BOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="297">
   <si>
     <t>Item #</t>
   </si>
@@ -198,18 +198,9 @@
     <t>LED1208-RA</t>
   </si>
   <si>
-    <t>M1, M2, M3, M4</t>
-  </si>
-  <si>
     <t>MOUNT-HOLE3.3</t>
   </si>
   <si>
-    <t>M5, M6, M7, M8</t>
-  </si>
-  <si>
-    <t>FIDUCIAL1X2</t>
-  </si>
-  <si>
     <t>Q1</t>
   </si>
   <si>
@@ -810,21 +801,12 @@
     <t>Standoff</t>
   </si>
   <si>
-    <t>8400K-ND</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
-    <t xml:space="preserve">HEX M/F 4-40 .375"L </t>
-  </si>
-  <si>
     <t>J4, SW1</t>
   </si>
   <si>
-    <t>NOTE: This part does not require assembling</t>
-  </si>
-  <si>
     <t>497-5235-1-ND</t>
   </si>
   <si>
@@ -919,13 +901,19 @@
   </si>
   <si>
     <t>R1, R12, R14, R211, R24, R25, R45, R451, R452, R453</t>
+  </si>
+  <si>
+    <t>7200K-ND</t>
+  </si>
+  <si>
+    <t>STANDOFF HEX M/F .375"L 4-40 BR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -972,8 +960,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -985,13 +981,8 @@
         <fgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1011,21 +1002,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1059,7 +1035,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1079,7 +1055,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1087,11 +1062,20 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1396,10 +1380,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L60"/>
+  <dimension ref="A1:L58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J55" sqref="J55"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H63" sqref="H63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1417,20 +1401,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
-        <v>272</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
+      <c r="A1" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
     </row>
     <row r="3" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -1467,7 +1451,7 @@
         <v>9</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1478,25 +1462,25 @@
         <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="I4" t="s">
         <v>135</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="I4" t="s">
-        <v>138</v>
       </c>
       <c r="J4" s="2">
         <v>2</v>
@@ -1523,19 +1507,19 @@
         <v>16</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>34</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="J5" s="3">
         <v>2</v>
@@ -1544,7 +1528,7 @@
         <v>0.16</v>
       </c>
       <c r="L5" s="4">
-        <f t="shared" ref="L5:L59" si="0">J5*K5</f>
+        <f t="shared" ref="L5:L57" si="0">J5*K5</f>
         <v>0.32</v>
       </c>
     </row>
@@ -1562,19 +1546,19 @@
         <v>16</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>34</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="I6" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="J6" s="2">
         <v>2</v>
@@ -1601,19 +1585,19 @@
         <v>16</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>34</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="I7" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="J7" s="2">
         <v>1</v>
@@ -1640,19 +1624,19 @@
         <v>16</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I8" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="J8" s="2">
         <v>5</v>
@@ -1679,19 +1663,19 @@
         <v>16</v>
       </c>
       <c r="E9" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="I9" t="s">
         <v>140</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="I9" t="s">
-        <v>143</v>
       </c>
       <c r="J9" s="2">
         <v>1</v>
@@ -1718,19 +1702,19 @@
         <v>16</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G10" s="6" t="s">
         <v>34</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="I10" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J10" s="2">
         <v>1</v>
@@ -1757,19 +1741,19 @@
         <v>16</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="G11" s="6" t="s">
         <v>34</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="I11" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="J11" s="2">
         <v>6</v>
@@ -1796,19 +1780,19 @@
         <v>16</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="G12" s="6" t="s">
         <v>34</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="I12" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="J12" s="2">
         <v>4</v>
@@ -1847,7 +1831,7 @@
         <v>35</v>
       </c>
       <c r="I13" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="J13" s="2">
         <v>1</v>
@@ -1886,7 +1870,7 @@
         <v>39</v>
       </c>
       <c r="I14" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="J14" s="2">
         <v>1</v>
@@ -1925,7 +1909,7 @@
         <v>44</v>
       </c>
       <c r="I15" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="J15" s="2">
         <v>1</v>
@@ -1943,7 +1927,7 @@
         <v>13</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>45</v>
@@ -1964,7 +1948,7 @@
         <v>48</v>
       </c>
       <c r="I16" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="J16" s="2">
         <v>2</v>
@@ -1991,7 +1975,7 @@
         <v>50</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>51</v>
@@ -2000,10 +1984,10 @@
         <v>34</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="I17" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="J17" s="2">
         <v>1</v>
@@ -2024,25 +2008,25 @@
         <v>52</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>53</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="I18" s="10" t="s">
-        <v>276</v>
+        <v>269</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>270</v>
       </c>
       <c r="J18" s="2">
         <v>1</v>
@@ -2060,28 +2044,28 @@
         <v>16</v>
       </c>
       <c r="B19" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="I19" s="9" t="s">
         <v>285</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>286</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="I19" s="10" t="s">
-        <v>291</v>
       </c>
       <c r="J19" s="2">
         <v>1</v>
@@ -2108,7 +2092,7 @@
         <v>56</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>57</v>
@@ -2120,7 +2104,7 @@
         <v>58</v>
       </c>
       <c r="I20" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="J20" s="2">
         <v>1</v>
@@ -2138,28 +2122,28 @@
         <v>18</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>59</v>
       </c>
       <c r="E21" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H21" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="F21" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>180</v>
-      </c>
       <c r="I21" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="J21" s="2">
         <v>1</v>
@@ -2177,28 +2161,28 @@
         <v>19</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>59</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="I22" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="J22" s="2">
         <v>1</v>
@@ -2216,22 +2200,38 @@
         <v>20</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
+        <v>62</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I23" t="s">
+        <v>183</v>
+      </c>
       <c r="J23" s="2">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="K23">
+        <v>0.76</v>
       </c>
       <c r="L23">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -2239,22 +2239,38 @@
         <v>21</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
+        <v>65</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I24" t="s">
+        <v>184</v>
+      </c>
       <c r="J24" s="2">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="K24">
+        <v>0.45</v>
       </c>
       <c r="L24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -2262,77 +2278,62 @@
         <v>22</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F25" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="I25" t="s">
         <v>185</v>
       </c>
-      <c r="G25" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="I25" t="s">
-        <v>186</v>
-      </c>
       <c r="J25" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K25">
-        <v>0.76</v>
+        <v>0.84</v>
       </c>
       <c r="L25">
         <f t="shared" si="0"/>
-        <v>0.76</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
+        <v>1.68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
         <v>23</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="I26" t="s">
-        <v>187</v>
-      </c>
-      <c r="J26" s="2">
-        <v>1</v>
-      </c>
-      <c r="K26">
-        <v>0.45</v>
-      </c>
-      <c r="L26">
-        <f t="shared" si="0"/>
-        <v>0.45</v>
+      <c r="B26" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="J26" s="3">
+        <v>5</v>
+      </c>
+      <c r="L26" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -2340,62 +2341,77 @@
         <v>24</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>71</v>
+        <v>294</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>71</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>72</v>
+        <v>187</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="I27" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="J27" s="2">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="K27">
-        <v>0.84</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="L27">
         <f t="shared" si="0"/>
-        <v>1.68</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="3">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
         <v>25</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>299</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D28" s="3" t="s">
+      <c r="B28" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="J28" s="3">
+      <c r="D28" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="I28" t="s">
+        <v>193</v>
+      </c>
+      <c r="J28" s="2">
         <v>5</v>
       </c>
-      <c r="L28" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="K28">
+        <v>1.32</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="0"/>
+        <v>6.6000000000000005</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -2403,38 +2419,38 @@
         <v>26</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>300</v>
+        <v>76</v>
       </c>
       <c r="C29" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="I29" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="J29" s="2">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="K29">
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="L29">
         <f t="shared" si="0"/>
-        <v>0.18</v>
+        <v>3.5999999999999997E-2</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -2442,38 +2458,38 @@
         <v>27</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
+      </c>
+      <c r="C30" s="2">
+        <v>22</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>72</v>
+        <v>187</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="I30" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="J30" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K30">
-        <v>1.32</v>
+        <v>2.3E-2</v>
       </c>
       <c r="L30">
         <f t="shared" si="0"/>
-        <v>6.6000000000000005</v>
+        <v>4.5999999999999999E-2</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -2481,38 +2497,38 @@
         <v>28</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>79</v>
+        <v>200</v>
       </c>
       <c r="C31" s="2">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="I31" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="J31" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K31">
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="L31">
         <f t="shared" si="0"/>
-        <v>3.5999999999999997E-2</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -2520,38 +2536,38 @@
         <v>29</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C32" s="2">
-        <v>22</v>
+        <v>330</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="I32" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="J32" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K32">
         <v>2.3E-2</v>
       </c>
       <c r="L32">
         <f t="shared" si="0"/>
-        <v>4.5999999999999999E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
@@ -2559,38 +2575,38 @@
         <v>30</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="C33" s="2">
-        <v>100</v>
+        <v>287</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>286</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>204</v>
+        <v>288</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="I33" t="s">
-        <v>206</v>
+        <v>289</v>
+      </c>
+      <c r="I33" s="11" t="s">
+        <v>290</v>
       </c>
       <c r="J33" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="K33">
-        <v>1.7999999999999999E-2</v>
+        <v>0.21</v>
       </c>
       <c r="L33">
         <f t="shared" si="0"/>
-        <v>0.09</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
@@ -2598,28 +2614,28 @@
         <v>31</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C34" s="2">
-        <v>330</v>
+        <v>80</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="F34" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="I34" t="s">
         <v>209</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="I34" t="s">
-        <v>208</v>
       </c>
       <c r="J34" s="2">
         <v>1</v>
@@ -2637,38 +2653,38 @@
         <v>32</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>293</v>
+        <v>72</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>292</v>
+        <v>73</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>294</v>
+        <v>210</v>
       </c>
       <c r="G35" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="I35" s="12" t="s">
-        <v>296</v>
+        <v>211</v>
+      </c>
+      <c r="I35" t="s">
+        <v>212</v>
       </c>
       <c r="J35" s="2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="K35">
-        <v>0.21</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="L35">
         <f t="shared" si="0"/>
-        <v>0.21</v>
+        <v>0.10799999999999998</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
@@ -2676,38 +2692,38 @@
         <v>33</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="E36" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>190</v>
-      </c>
       <c r="F36" s="2" t="s">
-        <v>210</v>
+        <v>85</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>211</v>
+        <v>86</v>
       </c>
       <c r="I36" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="J36" s="2">
         <v>1</v>
       </c>
       <c r="K36">
-        <v>2.3E-2</v>
+        <v>1</v>
       </c>
       <c r="L36">
         <f t="shared" si="0"/>
-        <v>2.3E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
@@ -2715,38 +2731,38 @@
         <v>34</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>75</v>
+        <v>292</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="G37" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="I37" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="J37" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="K37">
-        <v>1.7999999999999999E-2</v>
+        <v>2.3E-2</v>
       </c>
       <c r="L37">
         <f t="shared" si="0"/>
-        <v>0.10799999999999998</v>
+        <v>6.9000000000000006E-2</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
@@ -2754,38 +2770,38 @@
         <v>35</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>85</v>
+        <v>291</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>87</v>
+        <v>187</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>88</v>
+        <v>217</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>89</v>
+        <v>218</v>
       </c>
       <c r="I38" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="J38" s="2">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="K38">
-        <v>1</v>
+        <v>2.3E-2</v>
       </c>
       <c r="L38">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.253</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
@@ -2793,38 +2809,38 @@
         <v>36</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>298</v>
+        <v>87</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>190</v>
+        <v>220</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="G39" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="I39" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="J39" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K39">
-        <v>2.3E-2</v>
+        <v>5.45</v>
       </c>
       <c r="L39">
         <f t="shared" si="0"/>
-        <v>6.9000000000000006E-2</v>
+        <v>5.45</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
@@ -2832,116 +2848,116 @@
         <v>37</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>82</v>
+        <v>89</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>274</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>74</v>
+        <v>274</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>190</v>
+        <v>275</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>220</v>
+        <v>276</v>
       </c>
       <c r="G40" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="I40" t="s">
-        <v>222</v>
+        <v>277</v>
+      </c>
+      <c r="I40" s="9" t="s">
+        <v>278</v>
       </c>
       <c r="J40" s="2">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="K40">
-        <v>2.3E-2</v>
+        <v>0.29099999999999998</v>
       </c>
       <c r="L40">
-        <f t="shared" si="0"/>
-        <v>0.253</v>
+        <f t="shared" ref="L40" si="2">J40*K40</f>
+        <v>0.29099999999999998</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>38</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C41" s="2" t="s">
-        <v>91</v>
-      </c>
       <c r="D41" s="2" t="s">
-        <v>91</v>
+        <v>226</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
+      </c>
+      <c r="F41" s="2">
+        <v>5122</v>
       </c>
       <c r="G41" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>224</v>
+        <v>233</v>
       </c>
       <c r="I41" t="s">
-        <v>226</v>
+        <v>237</v>
       </c>
       <c r="J41" s="2">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="K41">
-        <v>5.45</v>
+        <v>0.38</v>
       </c>
       <c r="L41">
         <f t="shared" si="0"/>
-        <v>5.45</v>
+        <v>2.66</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>39</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C42" s="11" t="s">
-        <v>280</v>
+      <c r="B42" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>280</v>
+        <v>228</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>282</v>
+        <v>224</v>
+      </c>
+      <c r="F42" s="2">
+        <v>5121</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="I42" s="10" t="s">
-        <v>284</v>
+        <v>234</v>
+      </c>
+      <c r="I42" t="s">
+        <v>238</v>
       </c>
       <c r="J42" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K42">
-        <v>0.29099999999999998</v>
+        <v>0.38</v>
       </c>
       <c r="L42">
-        <f t="shared" ref="L42" si="2">J42*K42</f>
-        <v>0.29099999999999998</v>
+        <f t="shared" si="0"/>
+        <v>0.76</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
@@ -2949,38 +2965,38 @@
         <v>40</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="F43" s="2">
-        <v>5122</v>
+        <v>5005</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="I43" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="J43" s="2">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="K43">
-        <v>0.38</v>
+        <v>0.36</v>
       </c>
       <c r="L43">
         <f t="shared" si="0"/>
-        <v>2.66</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
@@ -2988,116 +3004,116 @@
         <v>41</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="F44" s="2">
-        <v>5121</v>
+        <v>5009</v>
       </c>
       <c r="G44" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="I44" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J44" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K44">
-        <v>0.38</v>
+        <v>0.36</v>
       </c>
       <c r="L44">
         <f t="shared" si="0"/>
-        <v>0.76</v>
+        <v>1.08</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>42</v>
       </c>
-      <c r="B45" s="7" t="s">
-        <v>232</v>
+      <c r="B45" s="1" t="s">
+        <v>91</v>
       </c>
       <c r="C45" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E45" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D45" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="F45" s="2">
-        <v>5005</v>
+      <c r="F45" s="2" t="s">
+        <v>94</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>238</v>
+        <v>95</v>
       </c>
       <c r="I45" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="J45" s="2">
         <v>1</v>
       </c>
       <c r="K45">
-        <v>0.36</v>
+        <v>3.78</v>
       </c>
       <c r="L45">
         <f t="shared" si="0"/>
-        <v>0.36</v>
+        <v>3.78</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>43</v>
       </c>
-      <c r="B46" s="7" t="s">
-        <v>234</v>
+      <c r="B46" s="1" t="s">
+        <v>96</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>235</v>
+        <v>97</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="F46" s="2">
-        <v>5009</v>
+        <v>98</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>99</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>239</v>
+        <v>100</v>
       </c>
       <c r="I46" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="J46" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K46">
-        <v>0.36</v>
+        <v>8.9499999999999993</v>
       </c>
       <c r="L46">
         <f t="shared" si="0"/>
-        <v>1.08</v>
+        <v>8.9499999999999993</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
@@ -3105,38 +3121,38 @@
         <v>44</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="I47" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J47" s="2">
         <v>1</v>
       </c>
       <c r="K47">
-        <v>3.78</v>
+        <v>4.51</v>
       </c>
       <c r="L47">
         <f t="shared" si="0"/>
-        <v>3.78</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
@@ -3144,38 +3160,38 @@
         <v>45</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>102</v>
+        <v>264</v>
       </c>
       <c r="G48" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>103</v>
+        <v>263</v>
       </c>
       <c r="I48" t="s">
-        <v>245</v>
+        <v>265</v>
       </c>
       <c r="J48" s="2">
         <v>1</v>
       </c>
       <c r="K48">
-        <v>8.9499999999999993</v>
+        <v>1</v>
       </c>
       <c r="L48">
         <f t="shared" si="0"/>
-        <v>8.9499999999999993</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
@@ -3183,38 +3199,38 @@
         <v>46</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="G49" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="I49" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="J49" s="2">
         <v>1</v>
       </c>
       <c r="K49">
-        <v>4.51</v>
+        <v>3.3</v>
       </c>
       <c r="L49">
         <f t="shared" si="0"/>
-        <v>4.51</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
@@ -3222,38 +3238,38 @@
         <v>47</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>270</v>
+        <v>112</v>
       </c>
       <c r="G50" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>269</v>
+        <v>114</v>
       </c>
       <c r="I50" t="s">
-        <v>271</v>
+        <v>245</v>
       </c>
       <c r="J50" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K50">
-        <v>1</v>
+        <v>0.88</v>
       </c>
       <c r="L50">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>1.76</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
@@ -3261,38 +3277,38 @@
         <v>48</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="G51" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="I51" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J51" s="2">
         <v>1</v>
       </c>
       <c r="K51">
-        <v>3.3</v>
+        <v>1.5</v>
       </c>
       <c r="L51">
         <f t="shared" si="0"/>
-        <v>3.3</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
@@ -3300,38 +3316,38 @@
         <v>49</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="G52" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="I52" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="J52" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K52">
-        <v>0.88</v>
+        <v>1.3</v>
       </c>
       <c r="L52">
         <f t="shared" si="0"/>
-        <v>1.76</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
@@ -3339,38 +3355,38 @@
         <v>50</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>118</v>
+        <v>273</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="G53" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="I53" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J53" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K53">
-        <v>1.5</v>
+        <v>1.68</v>
       </c>
       <c r="L53">
         <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>8.4</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
@@ -3378,116 +3394,114 @@
         <v>51</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>123</v>
+        <v>249</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>124</v>
+        <v>250</v>
       </c>
       <c r="G54" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>125</v>
+        <v>251</v>
       </c>
       <c r="I54" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="J54" s="2">
         <v>1</v>
       </c>
       <c r="K54">
-        <v>1.3</v>
+        <v>3.45</v>
       </c>
       <c r="L54">
         <f t="shared" si="0"/>
-        <v>1.3</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A55" s="2">
+        <v>3.45</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="3">
         <v>52</v>
       </c>
-      <c r="B55" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="G55" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H55" s="2" t="s">
+      <c r="B55" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="I55" t="s">
-        <v>251</v>
-      </c>
-      <c r="J55" s="2">
-        <v>5</v>
-      </c>
-      <c r="K55">
-        <v>1.68</v>
-      </c>
-      <c r="L55">
-        <f t="shared" si="0"/>
-        <v>8.4</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A56" s="2">
+      <c r="C55" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H55" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="I55" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="J55" s="3">
+        <v>1</v>
+      </c>
+      <c r="K55" s="4">
+        <v>1.26</v>
+      </c>
+      <c r="L55" s="4">
+        <f t="shared" si="0"/>
+        <v>1.26</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="3">
         <v>53</v>
       </c>
-      <c r="B56" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="F56" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="G56" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H56" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="I56" t="s">
-        <v>255</v>
-      </c>
-      <c r="J56" s="2">
-        <v>1</v>
-      </c>
-      <c r="K56">
-        <v>3.45</v>
-      </c>
-      <c r="L56">
-        <f t="shared" si="0"/>
-        <v>3.45</v>
+      <c r="B56" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="F56" s="3">
+        <v>585460</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="H56" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="I56"/>
+      <c r="J56" s="3">
+        <v>1</v>
+      </c>
+      <c r="K56" s="4">
+        <v>16.95</v>
+      </c>
+      <c r="L56" s="4">
+        <f t="shared" si="0"/>
+        <v>16.95</v>
       </c>
     </row>
     <row r="57" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -3495,129 +3509,51 @@
         <v>54</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="C57" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="C57" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="D57" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="E57" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="F57" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="G57" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="H57" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="I57" s="4" t="s">
-        <v>258</v>
-      </c>
-      <c r="J57" s="3">
-        <v>1</v>
+      <c r="D57" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="E57" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="F57" s="15">
+        <v>7200</v>
+      </c>
+      <c r="G57" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="H57" s="15" t="s">
+        <v>295</v>
+      </c>
+      <c r="I57" s="16" t="s">
+        <v>296</v>
+      </c>
+      <c r="J57" s="15">
+        <v>4</v>
       </c>
       <c r="K57" s="4">
-        <v>1.26</v>
+        <v>0.51500000000000001</v>
       </c>
       <c r="L57" s="4">
         <f t="shared" si="0"/>
-        <v>1.26</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="3">
-        <v>55</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>262</v>
-      </c>
-      <c r="E58" s="3" t="s">
+        <v>2.06</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I58" s="7" t="s">
         <v>261</v>
       </c>
-      <c r="F58" s="3">
-        <v>585460</v>
-      </c>
-      <c r="G58" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="H58" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="I58" s="9" t="s">
-        <v>268</v>
-      </c>
-      <c r="J58" s="3">
-        <v>1</v>
-      </c>
-      <c r="K58" s="4">
-        <v>16.95</v>
-      </c>
-      <c r="L58" s="4">
-        <f t="shared" si="0"/>
-        <v>16.95</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="3">
-        <v>56</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>263</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="F59" s="3">
-        <v>8400</v>
-      </c>
-      <c r="G59" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="H59" s="3" t="s">
-        <v>264</v>
-      </c>
-      <c r="I59" s="9" t="s">
-        <v>268</v>
-      </c>
-      <c r="J59" s="3">
-        <v>10</v>
-      </c>
-      <c r="K59" s="4">
-        <v>0.51500000000000001</v>
-      </c>
-      <c r="L59" s="4">
-        <f t="shared" si="0"/>
-        <v>5.15</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I60" s="7" t="s">
-        <v>265</v>
-      </c>
-      <c r="J60" s="2">
-        <f>SUM(J4:J59)</f>
-        <v>142</v>
-      </c>
-      <c r="L60">
-        <f>SUM(L4:L59)</f>
-        <v>108.18500000000003</v>
+      <c r="J58" s="2">
+        <f>SUM(J4:J57)</f>
+        <v>128</v>
+      </c>
+      <c r="L58">
+        <f>SUM(L4:L57)</f>
+        <v>105.09500000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed a type in BOM.
</commit_message>
<xml_diff>
--- a/hardware/PowerBoard/PowerBoard_BOM.xlsx
+++ b/hardware/PowerBoard/PowerBoard_BOM.xlsx
@@ -801,9 +801,6 @@
     <t>IC ESD PROTECTION LO CAP SOT23-6</t>
   </si>
   <si>
-    <t>Bill of Materials for 'Marote - Power Supply Board (Rev B)'</t>
-  </si>
-  <si>
     <t>CON-71741-0002</t>
   </si>
   <si>
@@ -892,6 +889,9 @@
   </si>
   <si>
     <t>STANDOFF HEX M/F .375"L 4-40 BR</t>
+  </si>
+  <si>
+    <t>Bill of Materials for 'Marmote - Power Supply Board (Rev B)'</t>
   </si>
 </sst>
 </file>
@@ -1367,8 +1367,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1387,7 +1387,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
-        <v>261</v>
+        <v>291</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -1993,25 +1993,25 @@
         <v>52</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>53</v>
       </c>
       <c r="F18" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H18" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="G18" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H18" s="2" t="s">
+      <c r="I18" s="9" t="s">
         <v>264</v>
-      </c>
-      <c r="I18" s="9" t="s">
-        <v>265</v>
       </c>
       <c r="J18" s="2">
         <v>1</v>
@@ -2029,28 +2029,28 @@
         <v>16</v>
       </c>
       <c r="B19" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="C19" s="10" t="s">
         <v>274</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="D19" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="F19" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="G19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H19" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="G19" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H19" s="2" t="s">
+      <c r="I19" s="9" t="s">
         <v>279</v>
-      </c>
-      <c r="I19" s="9" t="s">
-        <v>280</v>
       </c>
       <c r="J19" s="2">
         <v>1</v>
@@ -2107,7 +2107,7 @@
         <v>18</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>172</v>
@@ -2302,7 +2302,7 @@
         <v>23</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>11</v>
@@ -2326,7 +2326,7 @@
         <v>24</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C27" s="2">
         <v>0</v>
@@ -2365,7 +2365,7 @@
         <v>25</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>74</v>
@@ -2560,10 +2560,10 @@
         <v>30</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>71</v>
@@ -2572,16 +2572,16 @@
         <v>186</v>
       </c>
       <c r="F33" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H33" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="G33" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H33" s="2" t="s">
+      <c r="I33" s="11" t="s">
         <v>284</v>
-      </c>
-      <c r="I33" s="11" t="s">
-        <v>285</v>
       </c>
       <c r="J33" s="2">
         <v>1</v>
@@ -2716,7 +2716,7 @@
         <v>34</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>77</v>
@@ -2755,7 +2755,7 @@
         <v>35</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>79</v>
@@ -2836,25 +2836,25 @@
         <v>89</v>
       </c>
       <c r="C40" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="E40" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="D40" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="E40" s="2" t="s">
+      <c r="F40" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="F40" s="2" t="s">
+      <c r="G40" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H40" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="G40" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H40" s="2" t="s">
+      <c r="I40" s="9" t="s">
         <v>272</v>
-      </c>
-      <c r="I40" s="9" t="s">
-        <v>273</v>
       </c>
       <c r="J40" s="2">
         <v>1</v>
@@ -3340,7 +3340,7 @@
         <v>50</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>123</v>
@@ -3475,10 +3475,10 @@
         <v>34</v>
       </c>
       <c r="H56" s="13" t="s">
+        <v>289</v>
+      </c>
+      <c r="I56" s="14" t="s">
         <v>290</v>
-      </c>
-      <c r="I56" s="14" t="s">
-        <v>291</v>
       </c>
       <c r="J56" s="13">
         <v>4</v>

</xml_diff>

<commit_message>
- Some components had to be replaced with compatible parts (ONLY BOM WAS UPDATED, SCHEMATIC, COMPONENT LIBRARY, LAYOUT REMAINED UNCHANGED)
Resistors:
MCR03EZPJ000 => MCR03ERTJ000
MCR03EZPJ101 => MCR03ERTJ101
MCR03EZPJ472 => MCR03ERTJ472
MCR03EZPFX1002 => MCR03ERTF1002
MCR03EZPFX1003 => MCR03ERTF1003

Crystal:
ECS-160-8-36CKM => 
Digi-Key Part Number             887-1336-1-ND
Manufacturer                       TXC CORPORATION
Manufacturer Part Number           8Z-16.000MEEQ-T
Description                        CRYSTAL 16.000 MHZ 10PF SMD
</commit_message>
<xml_diff>
--- a/hardware/PowerBoard/PowerBoard_BOM.xlsx
+++ b/hardware/PowerBoard/PowerBoard_BOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="293">
   <si>
     <t>Item #</t>
   </si>
@@ -402,9 +402,6 @@
     <t>X1</t>
   </si>
   <si>
-    <t>ECX-2236</t>
-  </si>
-  <si>
     <t>X2</t>
   </si>
   <si>
@@ -579,9 +576,6 @@
     <t>Rohm</t>
   </si>
   <si>
-    <t>MCR03EZPJ000</t>
-  </si>
-  <si>
     <t>RHM0.0GCT-ND</t>
   </si>
   <si>
@@ -618,9 +612,6 @@
     <t>R22, R34, R35, R38, R39</t>
   </si>
   <si>
-    <t>MCR03EZPJ101</t>
-  </si>
-  <si>
     <t>RHM100GCT-ND</t>
   </si>
   <si>
@@ -645,9 +636,6 @@
     <t>RES 2.10K OHM 1/10W 1% 0603 SMD</t>
   </si>
   <si>
-    <t>MCR03EZPJ472</t>
-  </si>
-  <si>
     <t>RHM4.7KGCT-ND</t>
   </si>
   <si>
@@ -657,18 +645,12 @@
     <t>THERMISTOR NTC 10K OHM 5% 0603</t>
   </si>
   <si>
-    <t>MCR03EZPFX1002</t>
-  </si>
-  <si>
     <t>RHM10.0KHCT-ND</t>
   </si>
   <si>
     <t>RES 10.0K OHM 1/10W 1% 0603 SMD</t>
   </si>
   <si>
-    <t>MCR03EZPFX1003</t>
-  </si>
-  <si>
     <t>RHM100KHCT-ND</t>
   </si>
   <si>
@@ -765,15 +747,6 @@
     <t>ECS</t>
   </si>
   <si>
-    <t>ECS-160-8-36CKM</t>
-  </si>
-  <si>
-    <t>XC1552CT-ND</t>
-  </si>
-  <si>
-    <t>CRYSTAL 16.000 MHZ 8PF SMD</t>
-  </si>
-  <si>
     <t>ECS-.327-7-34B-TR</t>
   </si>
   <si>
@@ -892,6 +865,36 @@
   </si>
   <si>
     <t>Bill of Materials for 'Marmote - Power Supply Board (Rev B)'</t>
+  </si>
+  <si>
+    <t>MCR03ERTJ000</t>
+  </si>
+  <si>
+    <t>MCR03ERTJ101</t>
+  </si>
+  <si>
+    <t>MCR03ERTJ472</t>
+  </si>
+  <si>
+    <t>MCR03ERTF1002</t>
+  </si>
+  <si>
+    <t>MCR03ERTF1003</t>
+  </si>
+  <si>
+    <t>4-SMD, No Lead (DFN, LCC)</t>
+  </si>
+  <si>
+    <t>TXC CORPORATION</t>
+  </si>
+  <si>
+    <t>8Z-16.000MEEQ-T</t>
+  </si>
+  <si>
+    <t>887-1336-1-ND</t>
+  </si>
+  <si>
+    <t>CRYSTAL 16.000 MHZ 10PF SMD</t>
   </si>
 </sst>
 </file>
@@ -1367,8 +1370,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K54" sqref="K54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1387,7 +1390,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -1436,7 +1439,7 @@
         <v>9</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1447,25 +1450,25 @@
         <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="I4" t="s">
         <v>134</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="I4" t="s">
-        <v>135</v>
       </c>
       <c r="J4" s="2">
         <v>2</v>
@@ -1492,19 +1495,19 @@
         <v>16</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F5" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="G5" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>155</v>
-      </c>
       <c r="I5" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J5" s="3">
         <v>2</v>
@@ -1531,19 +1534,19 @@
         <v>16</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F6" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="G6" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>146</v>
-      </c>
       <c r="I6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J6" s="2">
         <v>2</v>
@@ -1570,19 +1573,19 @@
         <v>16</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F7" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="G7" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H7" s="2" t="s">
+      <c r="I7" t="s">
         <v>151</v>
-      </c>
-      <c r="I7" t="s">
-        <v>152</v>
       </c>
       <c r="J7" s="2">
         <v>1</v>
@@ -1609,19 +1612,19 @@
         <v>16</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F8" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H8" s="2" t="s">
+      <c r="I8" t="s">
         <v>142</v>
-      </c>
-      <c r="I8" t="s">
-        <v>143</v>
       </c>
       <c r="J8" s="2">
         <v>5</v>
@@ -1648,19 +1651,19 @@
         <v>16</v>
       </c>
       <c r="E9" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="G9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H9" s="2" t="s">
+      <c r="I9" t="s">
         <v>139</v>
-      </c>
-      <c r="I9" t="s">
-        <v>140</v>
       </c>
       <c r="J9" s="2">
         <v>1</v>
@@ -1687,19 +1690,19 @@
         <v>16</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F10" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="I10" t="s">
         <v>147</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="I10" t="s">
-        <v>148</v>
       </c>
       <c r="J10" s="2">
         <v>1</v>
@@ -1726,19 +1729,19 @@
         <v>16</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F11" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="G11" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>161</v>
-      </c>
       <c r="I11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J11" s="2">
         <v>6</v>
@@ -1765,19 +1768,19 @@
         <v>16</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F12" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H12" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="G12" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>158</v>
-      </c>
       <c r="I12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J12" s="2">
         <v>4</v>
@@ -1816,7 +1819,7 @@
         <v>35</v>
       </c>
       <c r="I13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J13" s="2">
         <v>1</v>
@@ -1855,7 +1858,7 @@
         <v>39</v>
       </c>
       <c r="I14" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J14" s="2">
         <v>1</v>
@@ -1894,7 +1897,7 @@
         <v>44</v>
       </c>
       <c r="I15" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J15" s="2">
         <v>1</v>
@@ -1912,7 +1915,7 @@
         <v>13</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>45</v>
@@ -1933,7 +1936,7 @@
         <v>48</v>
       </c>
       <c r="I16" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J16" s="2">
         <v>2</v>
@@ -1960,7 +1963,7 @@
         <v>50</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>51</v>
@@ -1969,10 +1972,10 @@
         <v>34</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I17" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J17" s="2">
         <v>1</v>
@@ -1993,25 +1996,25 @@
         <v>52</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>53</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="J18" s="2">
         <v>1</v>
@@ -2029,28 +2032,28 @@
         <v>16</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="I19" s="9" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
       <c r="J19" s="2">
         <v>1</v>
@@ -2077,7 +2080,7 @@
         <v>56</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>57</v>
@@ -2089,7 +2092,7 @@
         <v>58</v>
       </c>
       <c r="I20" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J20" s="2">
         <v>1</v>
@@ -2107,28 +2110,28 @@
         <v>18</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>59</v>
       </c>
       <c r="E21" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="F21" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="G21" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="I21" t="s">
         <v>175</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="I21" t="s">
-        <v>176</v>
       </c>
       <c r="J21" s="2">
         <v>1</v>
@@ -2146,28 +2149,28 @@
         <v>19</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>171</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>59</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H22" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="I22" t="s">
         <v>178</v>
-      </c>
-      <c r="I22" t="s">
-        <v>179</v>
       </c>
       <c r="J22" s="2">
         <v>1</v>
@@ -2197,7 +2200,7 @@
         <v>69</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>34</v>
@@ -2206,7 +2209,7 @@
         <v>63</v>
       </c>
       <c r="I23" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J23" s="2">
         <v>1</v>
@@ -2245,7 +2248,7 @@
         <v>66</v>
       </c>
       <c r="I24" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J24" s="2">
         <v>1</v>
@@ -2275,16 +2278,16 @@
         <v>69</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I25" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="J25" s="2">
         <v>2</v>
@@ -2302,7 +2305,7 @@
         <v>23</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>11</v>
@@ -2326,7 +2329,7 @@
         <v>24</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="C27" s="2">
         <v>0</v>
@@ -2335,19 +2338,19 @@
         <v>71</v>
       </c>
       <c r="E27" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H27" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="I27" t="s">
         <v>187</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="I27" t="s">
-        <v>189</v>
       </c>
       <c r="J27" s="2">
         <v>10</v>
@@ -2365,7 +2368,7 @@
         <v>25</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>74</v>
@@ -2377,16 +2380,16 @@
         <v>69</v>
       </c>
       <c r="F28" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="I28" t="s">
         <v>190</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="I28" t="s">
-        <v>192</v>
       </c>
       <c r="J28" s="2">
         <v>5</v>
@@ -2413,19 +2416,19 @@
         <v>71</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H29" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="I29" t="s">
         <v>193</v>
-      </c>
-      <c r="I29" t="s">
-        <v>195</v>
       </c>
       <c r="J29" s="2">
         <v>2</v>
@@ -2452,19 +2455,19 @@
         <v>71</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F30" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="I30" t="s">
         <v>196</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="I30" t="s">
-        <v>198</v>
       </c>
       <c r="J30" s="2">
         <v>2</v>
@@ -2482,7 +2485,7 @@
         <v>28</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C31" s="2">
         <v>100</v>
@@ -2491,19 +2494,19 @@
         <v>71</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>200</v>
+        <v>284</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="I31" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="J31" s="2">
         <v>5</v>
@@ -2530,19 +2533,19 @@
         <v>71</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="I32" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="J32" s="2">
         <v>1</v>
@@ -2560,28 +2563,28 @@
         <v>30</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>71</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="I33" s="11" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="J33" s="2">
         <v>1</v>
@@ -2608,19 +2611,19 @@
         <v>71</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="G34" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="I34" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="J34" s="2">
         <v>1</v>
@@ -2647,19 +2650,19 @@
         <v>71</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>209</v>
+        <v>285</v>
       </c>
       <c r="G35" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="I35" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J35" s="2">
         <v>6</v>
@@ -2698,7 +2701,7 @@
         <v>86</v>
       </c>
       <c r="I36" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="J36" s="2">
         <v>1</v>
@@ -2716,7 +2719,7 @@
         <v>34</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>77</v>
@@ -2725,19 +2728,19 @@
         <v>71</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>213</v>
+        <v>286</v>
       </c>
       <c r="G37" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="I37" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="J37" s="2">
         <v>3</v>
@@ -2755,7 +2758,7 @@
         <v>35</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>79</v>
@@ -2764,19 +2767,19 @@
         <v>71</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>216</v>
+        <v>287</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="I38" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="J38" s="2">
         <v>11</v>
@@ -2803,19 +2806,19 @@
         <v>88</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="G39" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="I39" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="J39" s="2">
         <v>1</v>
@@ -2836,25 +2839,25 @@
         <v>89</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="G40" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="I40" s="9" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="J40" s="2">
         <v>1</v>
@@ -2872,16 +2875,16 @@
         <v>38</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>90</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="F41" s="2">
         <v>5122</v>
@@ -2890,10 +2893,10 @@
         <v>34</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="I41" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="J41" s="2">
         <v>7</v>
@@ -2911,16 +2914,16 @@
         <v>39</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>90</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="F42" s="2">
         <v>5121</v>
@@ -2929,10 +2932,10 @@
         <v>34</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="I42" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="J42" s="2">
         <v>2</v>
@@ -2950,16 +2953,16 @@
         <v>40</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>90</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="F43" s="2">
         <v>5005</v>
@@ -2968,10 +2971,10 @@
         <v>34</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="I43" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="J43" s="2">
         <v>1</v>
@@ -2989,16 +2992,16 @@
         <v>41</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>90</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="F44" s="2">
         <v>5009</v>
@@ -3007,10 +3010,10 @@
         <v>34</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="I44" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="J44" s="2">
         <v>3</v>
@@ -3049,7 +3052,7 @@
         <v>95</v>
       </c>
       <c r="I45" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="J45" s="2">
         <v>1</v>
@@ -3088,7 +3091,7 @@
         <v>100</v>
       </c>
       <c r="I46" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="J46" s="2">
         <v>1</v>
@@ -3127,7 +3130,7 @@
         <v>104</v>
       </c>
       <c r="I47" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="J47" s="2">
         <v>1</v>
@@ -3157,16 +3160,16 @@
         <v>98</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="G48" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="I48" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="J48" s="2">
         <v>1</v>
@@ -3205,7 +3208,7 @@
         <v>110</v>
       </c>
       <c r="I49" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="J49" s="2">
         <v>1</v>
@@ -3244,7 +3247,7 @@
         <v>114</v>
       </c>
       <c r="I50" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="J50" s="2">
         <v>2</v>
@@ -3283,7 +3286,7 @@
         <v>117</v>
       </c>
       <c r="I51" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="J51" s="2">
         <v>1</v>
@@ -3322,7 +3325,7 @@
         <v>122</v>
       </c>
       <c r="I52" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="J52" s="2">
         <v>1</v>
@@ -3340,7 +3343,7 @@
         <v>50</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>123</v>
@@ -3361,7 +3364,7 @@
         <v>126</v>
       </c>
       <c r="I53" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="J53" s="2">
         <v>5</v>
@@ -3381,36 +3384,31 @@
       <c r="B54" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C54" s="2" t="s">
-        <v>128</v>
-      </c>
+      <c r="C54" s="2"/>
       <c r="D54" s="2" t="s">
-        <v>128</v>
+        <v>288</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>248</v>
+        <v>289</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>249</v>
+        <v>290</v>
       </c>
       <c r="G54" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>250</v>
+        <v>291</v>
       </c>
       <c r="I54" t="s">
-        <v>251</v>
+        <v>292</v>
       </c>
       <c r="J54" s="2">
         <v>1</v>
       </c>
-      <c r="K54">
-        <v>3.45</v>
-      </c>
       <c r="L54">
         <f t="shared" si="0"/>
-        <v>3.45</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -3418,28 +3416,28 @@
         <v>52</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="G55" s="3" t="s">
         <v>34</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="I55" s="4" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="J55" s="3">
         <v>1</v>
@@ -3457,7 +3455,7 @@
         <v>53</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="C56" s="12" t="s">
         <v>11</v>
@@ -3466,7 +3464,7 @@
         <v>60</v>
       </c>
       <c r="E56" s="13" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="F56" s="13">
         <v>7200</v>
@@ -3475,10 +3473,10 @@
         <v>34</v>
       </c>
       <c r="H56" s="13" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="I56" s="14" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="J56" s="13">
         <v>4</v>
@@ -3493,7 +3491,7 @@
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I57" s="7" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="J57" s="2">
         <f>SUM(J4:J56)</f>
@@ -3501,7 +3499,7 @@
       </c>
       <c r="L57">
         <f>SUM(L4:L56)</f>
-        <v>88.145000000000024</v>
+        <v>84.695000000000022</v>
       </c>
     </row>
   </sheetData>

</xml_diff>